<commit_message>
Finished EDA, pre-Feature Selection
</commit_message>
<xml_diff>
--- a/utility/data/HPSAdata/Hpsa_Find_Export (39).xlsx
+++ b/utility/data/HPSAdata/Hpsa_Find_Export (39).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsiu8\HPSA-Data\utility\data\HPSA data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsiu8\HPSA-Data\utility\data\HPSAdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065D947C-140F-4BA4-B592-6D1BA50D8A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D40F560-6DEF-441B-A0C1-654974FF0027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4101" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4101" uniqueCount="1396">
   <si>
     <t>data.HRSA.gov – HPSA Find</t>
   </si>
@@ -2519,9 +2519,6 @@
   </si>
   <si>
     <t>Federally Qualified Health Center Look-alike</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
   <si>
     <t>Careteam + Family Health and Specialty Care</t>
@@ -4742,8 +4739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A508" workbookViewId="0">
-      <selection activeCell="M528" sqref="M528"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="J319" sqref="J319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12797,8 +12794,8 @@
       <c r="I319" t="s">
         <v>21</v>
       </c>
-      <c r="J319" t="s">
-        <v>833</v>
+      <c r="J319" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="K319" t="s">
         <v>461</v>
@@ -12832,10 +12829,10 @@
     </row>
     <row r="321" spans="1:12">
       <c r="B321" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="C321" s="5" t="s">
         <v>834</v>
-      </c>
-      <c r="C321" s="5" t="s">
-        <v>835</v>
       </c>
       <c r="D321" s="5" t="s">
         <v>444</v>
@@ -12844,7 +12841,7 @@
         <v>49</v>
       </c>
       <c r="F321" s="5" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G321" s="5" t="s">
         <v>278</v>
@@ -12858,10 +12855,10 @@
         <v>13</v>
       </c>
       <c r="B322" t="s">
+        <v>836</v>
+      </c>
+      <c r="C322" t="s">
         <v>837</v>
-      </c>
-      <c r="C322" t="s">
-        <v>838</v>
       </c>
       <c r="D322" t="s">
         <v>436</v>
@@ -12888,7 +12885,7 @@
         <v>437</v>
       </c>
       <c r="L322" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="323" spans="1:12">
@@ -12916,19 +12913,19 @@
     </row>
     <row r="324" spans="1:12">
       <c r="B324" s="9" t="s">
+        <v>839</v>
+      </c>
+      <c r="C324" s="4" t="s">
         <v>840</v>
       </c>
-      <c r="C324" s="4" t="s">
+      <c r="D324" s="4" t="s">
         <v>841</v>
       </c>
-      <c r="D324" s="4" t="s">
+      <c r="E324" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F324" s="4" t="s">
         <v>842</v>
-      </c>
-      <c r="E324" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F324" s="4" t="s">
-        <v>843</v>
       </c>
       <c r="G324" s="4" t="s">
         <v>264</v>
@@ -12939,10 +12936,10 @@
     </row>
     <row r="325" spans="1:12">
       <c r="B325" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="C325" t="s">
         <v>844</v>
-      </c>
-      <c r="C325" t="s">
-        <v>845</v>
       </c>
       <c r="D325" t="s">
         <v>153</v>
@@ -12951,7 +12948,7 @@
         <v>49</v>
       </c>
       <c r="F325" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G325" t="s">
         <v>155</v>
@@ -12962,10 +12959,10 @@
     </row>
     <row r="326" spans="1:12">
       <c r="B326" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="C326" t="s">
         <v>847</v>
-      </c>
-      <c r="C326" t="s">
-        <v>848</v>
       </c>
       <c r="D326" t="s">
         <v>136</v>
@@ -12974,7 +12971,7 @@
         <v>49</v>
       </c>
       <c r="F326" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G326" t="s">
         <v>138</v>
@@ -12985,19 +12982,19 @@
     </row>
     <row r="327" spans="1:12">
       <c r="B327" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="C327" t="s">
         <v>850</v>
       </c>
-      <c r="C327" t="s">
+      <c r="D327" t="s">
         <v>851</v>
       </c>
-      <c r="D327" t="s">
+      <c r="E327" t="s">
+        <v>49</v>
+      </c>
+      <c r="F327" t="s">
         <v>852</v>
-      </c>
-      <c r="E327" t="s">
-        <v>49</v>
-      </c>
-      <c r="F327" t="s">
-        <v>853</v>
       </c>
       <c r="G327" t="s">
         <v>234</v>
@@ -13008,10 +13005,10 @@
     </row>
     <row r="328" spans="1:12">
       <c r="B328" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="C328" t="s">
         <v>854</v>
-      </c>
-      <c r="C328" t="s">
-        <v>855</v>
       </c>
       <c r="D328" t="s">
         <v>234</v>
@@ -13020,7 +13017,7 @@
         <v>49</v>
       </c>
       <c r="F328" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G328" t="s">
         <v>234</v>
@@ -13031,10 +13028,10 @@
     </row>
     <row r="329" spans="1:12">
       <c r="B329" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="C329" t="s">
         <v>857</v>
-      </c>
-      <c r="C329" t="s">
-        <v>858</v>
       </c>
       <c r="D329" t="s">
         <v>251</v>
@@ -13043,7 +13040,7 @@
         <v>49</v>
       </c>
       <c r="F329" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G329" t="s">
         <v>251</v>
@@ -13054,10 +13051,10 @@
     </row>
     <row r="330" spans="1:12">
       <c r="B330" s="10" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C330" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D330" t="s">
         <v>251</v>
@@ -13066,7 +13063,7 @@
         <v>49</v>
       </c>
       <c r="F330" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G330" t="s">
         <v>251</v>
@@ -13077,19 +13074,19 @@
     </row>
     <row r="331" spans="1:12">
       <c r="B331" s="10" t="s">
+        <v>861</v>
+      </c>
+      <c r="C331" t="s">
         <v>862</v>
       </c>
-      <c r="C331" t="s">
+      <c r="D331" t="s">
+        <v>841</v>
+      </c>
+      <c r="E331" t="s">
+        <v>49</v>
+      </c>
+      <c r="F331" t="s">
         <v>863</v>
-      </c>
-      <c r="D331" t="s">
-        <v>842</v>
-      </c>
-      <c r="E331" t="s">
-        <v>49</v>
-      </c>
-      <c r="F331" t="s">
-        <v>864</v>
       </c>
       <c r="G331" t="s">
         <v>264</v>
@@ -13100,19 +13097,19 @@
     </row>
     <row r="332" spans="1:12">
       <c r="B332" s="10" t="s">
+        <v>864</v>
+      </c>
+      <c r="C332" t="s">
         <v>865</v>
       </c>
-      <c r="C332" t="s">
+      <c r="D332" t="s">
         <v>866</v>
       </c>
-      <c r="D332" t="s">
+      <c r="E332" t="s">
+        <v>49</v>
+      </c>
+      <c r="F332" t="s">
         <v>867</v>
-      </c>
-      <c r="E332" t="s">
-        <v>49</v>
-      </c>
-      <c r="F332" t="s">
-        <v>868</v>
       </c>
       <c r="G332" t="s">
         <v>251</v>
@@ -13123,19 +13120,19 @@
     </row>
     <row r="333" spans="1:12">
       <c r="B333" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="C333" t="s">
         <v>869</v>
       </c>
-      <c r="C333" t="s">
+      <c r="D333" t="s">
         <v>870</v>
       </c>
-      <c r="D333" t="s">
+      <c r="E333" t="s">
+        <v>49</v>
+      </c>
+      <c r="F333" t="s">
         <v>871</v>
-      </c>
-      <c r="E333" t="s">
-        <v>49</v>
-      </c>
-      <c r="F333" t="s">
-        <v>872</v>
       </c>
       <c r="G333" t="s">
         <v>155</v>
@@ -13146,19 +13143,19 @@
     </row>
     <row r="334" spans="1:12">
       <c r="B334" s="10" t="s">
+        <v>872</v>
+      </c>
+      <c r="C334" t="s">
         <v>873</v>
       </c>
-      <c r="C334" t="s">
+      <c r="D334" t="s">
         <v>874</v>
       </c>
-      <c r="D334" t="s">
+      <c r="E334" t="s">
+        <v>49</v>
+      </c>
+      <c r="F334" t="s">
         <v>875</v>
-      </c>
-      <c r="E334" t="s">
-        <v>49</v>
-      </c>
-      <c r="F334" t="s">
-        <v>876</v>
       </c>
       <c r="G334" t="s">
         <v>264</v>
@@ -13169,10 +13166,10 @@
     </row>
     <row r="335" spans="1:12">
       <c r="B335" s="10" t="s">
+        <v>876</v>
+      </c>
+      <c r="C335" t="s">
         <v>877</v>
-      </c>
-      <c r="C335" t="s">
-        <v>878</v>
       </c>
       <c r="D335" t="s">
         <v>153</v>
@@ -13181,7 +13178,7 @@
         <v>49</v>
       </c>
       <c r="F335" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G335" t="s">
         <v>155</v>
@@ -13192,10 +13189,10 @@
     </row>
     <row r="336" spans="1:12">
       <c r="B336" s="10" t="s">
+        <v>879</v>
+      </c>
+      <c r="C336" t="s">
         <v>880</v>
-      </c>
-      <c r="C336" t="s">
-        <v>881</v>
       </c>
       <c r="D336" t="s">
         <v>153</v>
@@ -13204,7 +13201,7 @@
         <v>49</v>
       </c>
       <c r="F336" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G336" t="s">
         <v>155</v>
@@ -13215,10 +13212,10 @@
     </row>
     <row r="337" spans="1:12">
       <c r="B337" s="10" t="s">
+        <v>882</v>
+      </c>
+      <c r="C337" t="s">
         <v>883</v>
-      </c>
-      <c r="C337" t="s">
-        <v>884</v>
       </c>
       <c r="D337" t="s">
         <v>136</v>
@@ -13227,7 +13224,7 @@
         <v>49</v>
       </c>
       <c r="F337" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G337" t="s">
         <v>138</v>
@@ -13238,19 +13235,19 @@
     </row>
     <row r="338" spans="1:12">
       <c r="B338" s="10" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C338" t="s">
+        <v>840</v>
+      </c>
+      <c r="D338" t="s">
         <v>841</v>
       </c>
-      <c r="D338" t="s">
+      <c r="E338" t="s">
+        <v>49</v>
+      </c>
+      <c r="F338" t="s">
         <v>842</v>
-      </c>
-      <c r="E338" t="s">
-        <v>49</v>
-      </c>
-      <c r="F338" t="s">
-        <v>843</v>
       </c>
       <c r="G338" t="s">
         <v>264</v>
@@ -13261,19 +13258,19 @@
     </row>
     <row r="339" spans="1:12">
       <c r="B339" s="10" t="s">
+        <v>886</v>
+      </c>
+      <c r="C339" t="s">
         <v>887</v>
       </c>
-      <c r="C339" t="s">
+      <c r="D339" t="s">
         <v>888</v>
       </c>
-      <c r="D339" t="s">
+      <c r="E339" t="s">
+        <v>49</v>
+      </c>
+      <c r="F339" t="s">
         <v>889</v>
-      </c>
-      <c r="E339" t="s">
-        <v>49</v>
-      </c>
-      <c r="F339" t="s">
-        <v>890</v>
       </c>
       <c r="G339" t="s">
         <v>251</v>
@@ -13284,19 +13281,19 @@
     </row>
     <row r="340" spans="1:12">
       <c r="B340" s="10" t="s">
+        <v>890</v>
+      </c>
+      <c r="C340" t="s">
         <v>891</v>
       </c>
-      <c r="C340" t="s">
+      <c r="D340" t="s">
+        <v>874</v>
+      </c>
+      <c r="E340" t="s">
+        <v>49</v>
+      </c>
+      <c r="F340" t="s">
         <v>892</v>
-      </c>
-      <c r="D340" t="s">
-        <v>875</v>
-      </c>
-      <c r="E340" t="s">
-        <v>49</v>
-      </c>
-      <c r="F340" t="s">
-        <v>893</v>
       </c>
       <c r="G340" t="s">
         <v>264</v>
@@ -13307,19 +13304,19 @@
     </row>
     <row r="341" spans="1:12">
       <c r="B341" s="10" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C341" t="s">
+        <v>891</v>
+      </c>
+      <c r="D341" t="s">
+        <v>874</v>
+      </c>
+      <c r="E341" t="s">
+        <v>49</v>
+      </c>
+      <c r="F341" t="s">
         <v>892</v>
-      </c>
-      <c r="D341" t="s">
-        <v>875</v>
-      </c>
-      <c r="E341" t="s">
-        <v>49</v>
-      </c>
-      <c r="F341" t="s">
-        <v>893</v>
       </c>
       <c r="G341" t="s">
         <v>264</v>
@@ -13330,19 +13327,19 @@
     </row>
     <row r="342" spans="1:12">
       <c r="B342" s="10" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C342" t="s">
+        <v>891</v>
+      </c>
+      <c r="D342" t="s">
+        <v>874</v>
+      </c>
+      <c r="E342" t="s">
+        <v>49</v>
+      </c>
+      <c r="F342" t="s">
         <v>892</v>
-      </c>
-      <c r="D342" t="s">
-        <v>875</v>
-      </c>
-      <c r="E342" t="s">
-        <v>49</v>
-      </c>
-      <c r="F342" t="s">
-        <v>893</v>
       </c>
       <c r="G342" t="s">
         <v>264</v>
@@ -13353,19 +13350,19 @@
     </row>
     <row r="343" spans="1:12">
       <c r="B343" s="10" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C343" t="s">
+        <v>840</v>
+      </c>
+      <c r="D343" t="s">
         <v>841</v>
       </c>
-      <c r="D343" t="s">
+      <c r="E343" t="s">
+        <v>49</v>
+      </c>
+      <c r="F343" t="s">
         <v>842</v>
-      </c>
-      <c r="E343" t="s">
-        <v>49</v>
-      </c>
-      <c r="F343" t="s">
-        <v>843</v>
       </c>
       <c r="G343" t="s">
         <v>264</v>
@@ -13376,19 +13373,19 @@
     </row>
     <row r="344" spans="1:12">
       <c r="B344" s="11" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C344" s="8" t="s">
+        <v>840</v>
+      </c>
+      <c r="D344" s="8" t="s">
         <v>841</v>
       </c>
-      <c r="D344" s="8" t="s">
+      <c r="E344" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F344" s="8" t="s">
         <v>842</v>
-      </c>
-      <c r="E344" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F344" s="8" t="s">
-        <v>843</v>
       </c>
       <c r="G344" s="8" t="s">
         <v>264</v>
@@ -13402,10 +13399,10 @@
         <v>13</v>
       </c>
       <c r="B345" t="s">
+        <v>897</v>
+      </c>
+      <c r="C345" t="s">
         <v>898</v>
-      </c>
-      <c r="C345" t="s">
-        <v>899</v>
       </c>
       <c r="D345" t="s">
         <v>158</v>
@@ -13432,7 +13429,7 @@
         <v>437</v>
       </c>
       <c r="L345" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="346" spans="1:12">
@@ -13460,10 +13457,10 @@
     </row>
     <row r="347" spans="1:12">
       <c r="B347" s="6" t="s">
+        <v>898</v>
+      </c>
+      <c r="C347" s="5" t="s">
         <v>899</v>
-      </c>
-      <c r="C347" s="5" t="s">
-        <v>900</v>
       </c>
       <c r="D347" s="5" t="s">
         <v>181</v>
@@ -13472,7 +13469,7 @@
         <v>49</v>
       </c>
       <c r="F347" s="5" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G347" s="5" t="s">
         <v>181</v>
@@ -13486,10 +13483,10 @@
         <v>13</v>
       </c>
       <c r="B348" t="s">
+        <v>901</v>
+      </c>
+      <c r="C348" t="s">
         <v>902</v>
-      </c>
-      <c r="C348" t="s">
-        <v>903</v>
       </c>
       <c r="D348" t="s">
         <v>436</v>
@@ -13516,7 +13513,7 @@
         <v>437</v>
       </c>
       <c r="L348" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="349" spans="1:12">
@@ -13544,10 +13541,10 @@
     </row>
     <row r="350" spans="1:12">
       <c r="B350" s="9" t="s">
+        <v>903</v>
+      </c>
+      <c r="C350" s="4" t="s">
         <v>904</v>
-      </c>
-      <c r="C350" s="4" t="s">
-        <v>905</v>
       </c>
       <c r="D350" s="4" t="s">
         <v>48</v>
@@ -13556,7 +13553,7 @@
         <v>49</v>
       </c>
       <c r="F350" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="G350" s="4" t="s">
         <v>51</v>
@@ -13567,22 +13564,22 @@
     </row>
     <row r="351" spans="1:12">
       <c r="B351" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="C351" t="s">
         <v>907</v>
       </c>
-      <c r="C351" t="s">
+      <c r="D351" t="s">
         <v>908</v>
       </c>
-      <c r="D351" t="s">
+      <c r="E351" t="s">
+        <v>49</v>
+      </c>
+      <c r="F351" t="s">
         <v>909</v>
       </c>
-      <c r="E351" t="s">
-        <v>49</v>
-      </c>
-      <c r="F351" t="s">
+      <c r="G351" t="s">
         <v>910</v>
-      </c>
-      <c r="G351" t="s">
-        <v>911</v>
       </c>
       <c r="H351" s="13" t="s">
         <v>39</v>
@@ -13590,22 +13587,22 @@
     </row>
     <row r="352" spans="1:12">
       <c r="B352" s="10" t="s">
+        <v>911</v>
+      </c>
+      <c r="C352" t="s">
         <v>912</v>
       </c>
-      <c r="C352" t="s">
+      <c r="D352" t="s">
         <v>913</v>
       </c>
-      <c r="D352" t="s">
+      <c r="E352" t="s">
+        <v>49</v>
+      </c>
+      <c r="F352" t="s">
         <v>914</v>
       </c>
-      <c r="E352" t="s">
-        <v>49</v>
-      </c>
-      <c r="F352" t="s">
-        <v>915</v>
-      </c>
       <c r="G352" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H352" s="13" t="s">
         <v>39</v>
@@ -13613,22 +13610,22 @@
     </row>
     <row r="353" spans="2:8">
       <c r="B353" s="10" t="s">
+        <v>915</v>
+      </c>
+      <c r="C353" t="s">
         <v>916</v>
       </c>
-      <c r="C353" t="s">
+      <c r="D353" t="s">
+        <v>908</v>
+      </c>
+      <c r="E353" t="s">
+        <v>49</v>
+      </c>
+      <c r="F353" t="s">
         <v>917</v>
       </c>
-      <c r="D353" t="s">
-        <v>909</v>
-      </c>
-      <c r="E353" t="s">
-        <v>49</v>
-      </c>
-      <c r="F353" t="s">
-        <v>918</v>
-      </c>
       <c r="G353" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H353" s="13" t="s">
         <v>39</v>
@@ -13636,10 +13633,10 @@
     </row>
     <row r="354" spans="2:8">
       <c r="B354" s="10" t="s">
+        <v>918</v>
+      </c>
+      <c r="C354" t="s">
         <v>919</v>
-      </c>
-      <c r="C354" t="s">
-        <v>920</v>
       </c>
       <c r="D354" t="s">
         <v>48</v>
@@ -13648,7 +13645,7 @@
         <v>49</v>
       </c>
       <c r="F354" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G354" t="s">
         <v>51</v>
@@ -13659,10 +13656,10 @@
     </row>
     <row r="355" spans="2:8">
       <c r="B355" s="10" t="s">
+        <v>921</v>
+      </c>
+      <c r="C355" t="s">
         <v>922</v>
-      </c>
-      <c r="C355" t="s">
-        <v>923</v>
       </c>
       <c r="D355" t="s">
         <v>48</v>
@@ -13671,7 +13668,7 @@
         <v>49</v>
       </c>
       <c r="F355" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G355" t="s">
         <v>51</v>
@@ -13682,10 +13679,10 @@
     </row>
     <row r="356" spans="2:8">
       <c r="B356" s="10" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C356" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D356" t="s">
         <v>48</v>
@@ -13694,7 +13691,7 @@
         <v>49</v>
       </c>
       <c r="F356" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G356" t="s">
         <v>51</v>
@@ -13705,19 +13702,19 @@
     </row>
     <row r="357" spans="2:8">
       <c r="B357" s="10" t="s">
+        <v>925</v>
+      </c>
+      <c r="C357" t="s">
         <v>926</v>
       </c>
-      <c r="C357" t="s">
+      <c r="D357" t="s">
         <v>927</v>
       </c>
-      <c r="D357" t="s">
+      <c r="E357" t="s">
+        <v>49</v>
+      </c>
+      <c r="F357" t="s">
         <v>928</v>
-      </c>
-      <c r="E357" t="s">
-        <v>49</v>
-      </c>
-      <c r="F357" t="s">
-        <v>929</v>
       </c>
       <c r="G357" t="s">
         <v>51</v>
@@ -13728,10 +13725,10 @@
     </row>
     <row r="358" spans="2:8">
       <c r="B358" s="10" t="s">
+        <v>929</v>
+      </c>
+      <c r="C358" t="s">
         <v>930</v>
-      </c>
-      <c r="C358" t="s">
-        <v>931</v>
       </c>
       <c r="D358" t="s">
         <v>48</v>
@@ -13740,7 +13737,7 @@
         <v>49</v>
       </c>
       <c r="F358" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G358" t="s">
         <v>51</v>
@@ -13751,10 +13748,10 @@
     </row>
     <row r="359" spans="2:8">
       <c r="B359" s="10" t="s">
+        <v>931</v>
+      </c>
+      <c r="C359" t="s">
         <v>932</v>
-      </c>
-      <c r="C359" t="s">
-        <v>933</v>
       </c>
       <c r="D359" t="s">
         <v>48</v>
@@ -13763,7 +13760,7 @@
         <v>49</v>
       </c>
       <c r="F359" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G359" t="s">
         <v>51</v>
@@ -13774,10 +13771,10 @@
     </row>
     <row r="360" spans="2:8">
       <c r="B360" s="10" t="s">
+        <v>933</v>
+      </c>
+      <c r="C360" t="s">
         <v>934</v>
-      </c>
-      <c r="C360" t="s">
-        <v>935</v>
       </c>
       <c r="D360" t="s">
         <v>48</v>
@@ -13786,10 +13783,10 @@
         <v>49</v>
       </c>
       <c r="F360" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="G360" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H360" s="13" t="s">
         <v>39</v>
@@ -13797,10 +13794,10 @@
     </row>
     <row r="361" spans="2:8">
       <c r="B361" s="10" t="s">
+        <v>936</v>
+      </c>
+      <c r="C361" t="s">
         <v>937</v>
-      </c>
-      <c r="C361" t="s">
-        <v>938</v>
       </c>
       <c r="D361" t="s">
         <v>48</v>
@@ -13809,7 +13806,7 @@
         <v>49</v>
       </c>
       <c r="F361" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="G361" t="s">
         <v>51</v>
@@ -13820,10 +13817,10 @@
     </row>
     <row r="362" spans="2:8">
       <c r="B362" s="10" t="s">
+        <v>939</v>
+      </c>
+      <c r="C362" t="s">
         <v>940</v>
-      </c>
-      <c r="C362" t="s">
-        <v>941</v>
       </c>
       <c r="D362" t="s">
         <v>48</v>
@@ -13832,7 +13829,7 @@
         <v>49</v>
       </c>
       <c r="F362" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G362" t="s">
         <v>51</v>
@@ -13843,10 +13840,10 @@
     </row>
     <row r="363" spans="2:8">
       <c r="B363" s="10" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C363" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D363" t="s">
         <v>48</v>
@@ -13855,7 +13852,7 @@
         <v>49</v>
       </c>
       <c r="F363" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G363" t="s">
         <v>51</v>
@@ -13866,10 +13863,10 @@
     </row>
     <row r="364" spans="2:8">
       <c r="B364" s="10" t="s">
+        <v>942</v>
+      </c>
+      <c r="C364" t="s">
         <v>943</v>
-      </c>
-      <c r="C364" t="s">
-        <v>944</v>
       </c>
       <c r="D364" t="s">
         <v>48</v>
@@ -13878,7 +13875,7 @@
         <v>49</v>
       </c>
       <c r="F364" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="G364" t="s">
         <v>51</v>
@@ -13889,19 +13886,19 @@
     </row>
     <row r="365" spans="2:8">
       <c r="B365" s="10" t="s">
+        <v>944</v>
+      </c>
+      <c r="C365" t="s">
         <v>945</v>
       </c>
-      <c r="C365" t="s">
+      <c r="D365" t="s">
         <v>946</v>
       </c>
-      <c r="D365" t="s">
+      <c r="E365" t="s">
+        <v>49</v>
+      </c>
+      <c r="F365" t="s">
         <v>947</v>
-      </c>
-      <c r="E365" t="s">
-        <v>49</v>
-      </c>
-      <c r="F365" t="s">
-        <v>948</v>
       </c>
       <c r="G365" t="s">
         <v>271</v>
@@ -13912,10 +13909,10 @@
     </row>
     <row r="366" spans="2:8">
       <c r="B366" s="10" t="s">
+        <v>948</v>
+      </c>
+      <c r="C366" t="s">
         <v>949</v>
-      </c>
-      <c r="C366" t="s">
-        <v>950</v>
       </c>
       <c r="D366" t="s">
         <v>48</v>
@@ -13924,7 +13921,7 @@
         <v>49</v>
       </c>
       <c r="F366" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G366" t="s">
         <v>51</v>
@@ -13935,10 +13932,10 @@
     </row>
     <row r="367" spans="2:8">
       <c r="B367" s="10" t="s">
+        <v>951</v>
+      </c>
+      <c r="C367" t="s">
         <v>952</v>
-      </c>
-      <c r="C367" t="s">
-        <v>953</v>
       </c>
       <c r="D367" t="s">
         <v>48</v>
@@ -13947,7 +13944,7 @@
         <v>49</v>
       </c>
       <c r="F367" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G367" t="s">
         <v>51</v>
@@ -13958,19 +13955,19 @@
     </row>
     <row r="368" spans="2:8">
       <c r="B368" s="10" t="s">
+        <v>954</v>
+      </c>
+      <c r="C368" t="s">
         <v>955</v>
       </c>
-      <c r="C368" t="s">
+      <c r="D368" t="s">
         <v>956</v>
       </c>
-      <c r="D368" t="s">
+      <c r="E368" t="s">
+        <v>49</v>
+      </c>
+      <c r="F368" t="s">
         <v>957</v>
-      </c>
-      <c r="E368" t="s">
-        <v>49</v>
-      </c>
-      <c r="F368" t="s">
-        <v>958</v>
       </c>
       <c r="G368" t="s">
         <v>51</v>
@@ -13981,19 +13978,19 @@
     </row>
     <row r="369" spans="1:12">
       <c r="B369" s="10" t="s">
+        <v>958</v>
+      </c>
+      <c r="C369" t="s">
         <v>959</v>
       </c>
-      <c r="C369" t="s">
+      <c r="D369" t="s">
         <v>960</v>
       </c>
-      <c r="D369" t="s">
+      <c r="E369" t="s">
+        <v>49</v>
+      </c>
+      <c r="F369" t="s">
         <v>961</v>
-      </c>
-      <c r="E369" t="s">
-        <v>49</v>
-      </c>
-      <c r="F369" t="s">
-        <v>962</v>
       </c>
       <c r="G369" t="s">
         <v>271</v>
@@ -14004,19 +14001,19 @@
     </row>
     <row r="370" spans="1:12">
       <c r="B370" s="10" t="s">
+        <v>962</v>
+      </c>
+      <c r="C370" t="s">
         <v>963</v>
       </c>
-      <c r="C370" t="s">
+      <c r="D370" t="s">
         <v>964</v>
       </c>
-      <c r="D370" t="s">
+      <c r="E370" t="s">
+        <v>49</v>
+      </c>
+      <c r="F370" t="s">
         <v>965</v>
-      </c>
-      <c r="E370" t="s">
-        <v>49</v>
-      </c>
-      <c r="F370" t="s">
-        <v>966</v>
       </c>
       <c r="G370" t="s">
         <v>271</v>
@@ -14027,19 +14024,19 @@
     </row>
     <row r="371" spans="1:12">
       <c r="B371" s="10" t="s">
+        <v>966</v>
+      </c>
+      <c r="C371" t="s">
         <v>967</v>
       </c>
-      <c r="C371" t="s">
+      <c r="D371" t="s">
         <v>968</v>
       </c>
-      <c r="D371" t="s">
+      <c r="E371" t="s">
+        <v>49</v>
+      </c>
+      <c r="F371" t="s">
         <v>969</v>
-      </c>
-      <c r="E371" t="s">
-        <v>49</v>
-      </c>
-      <c r="F371" t="s">
-        <v>970</v>
       </c>
       <c r="G371" t="s">
         <v>397</v>
@@ -14050,22 +14047,22 @@
     </row>
     <row r="372" spans="1:12">
       <c r="B372" s="10" t="s">
+        <v>970</v>
+      </c>
+      <c r="C372" t="s">
         <v>971</v>
       </c>
-      <c r="C372" t="s">
+      <c r="D372" t="s">
         <v>972</v>
       </c>
-      <c r="D372" t="s">
+      <c r="E372" t="s">
+        <v>49</v>
+      </c>
+      <c r="F372" t="s">
         <v>973</v>
       </c>
-      <c r="E372" t="s">
-        <v>49</v>
-      </c>
-      <c r="F372" t="s">
-        <v>974</v>
-      </c>
       <c r="G372" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H372" s="13" t="s">
         <v>39</v>
@@ -14073,10 +14070,10 @@
     </row>
     <row r="373" spans="1:12">
       <c r="B373" s="10" t="s">
+        <v>974</v>
+      </c>
+      <c r="C373" t="s">
         <v>975</v>
-      </c>
-      <c r="C373" t="s">
-        <v>976</v>
       </c>
       <c r="D373" t="s">
         <v>397</v>
@@ -14085,7 +14082,7 @@
         <v>49</v>
       </c>
       <c r="F373" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="G373" t="s">
         <v>397</v>
@@ -14096,22 +14093,22 @@
     </row>
     <row r="374" spans="1:12">
       <c r="B374" s="10" t="s">
+        <v>977</v>
+      </c>
+      <c r="C374" t="s">
         <v>978</v>
       </c>
-      <c r="C374" t="s">
+      <c r="D374" t="s">
         <v>979</v>
       </c>
-      <c r="D374" t="s">
+      <c r="E374" t="s">
+        <v>49</v>
+      </c>
+      <c r="F374" t="s">
         <v>980</v>
       </c>
-      <c r="E374" t="s">
-        <v>49</v>
-      </c>
-      <c r="F374" t="s">
-        <v>981</v>
-      </c>
       <c r="G374" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H374" s="13" t="s">
         <v>39</v>
@@ -14119,19 +14116,19 @@
     </row>
     <row r="375" spans="1:12">
       <c r="B375" s="10" t="s">
+        <v>981</v>
+      </c>
+      <c r="C375" t="s">
         <v>982</v>
       </c>
-      <c r="C375" t="s">
+      <c r="D375" t="s">
         <v>983</v>
       </c>
-      <c r="D375" t="s">
+      <c r="E375" t="s">
+        <v>49</v>
+      </c>
+      <c r="F375" t="s">
         <v>984</v>
-      </c>
-      <c r="E375" t="s">
-        <v>49</v>
-      </c>
-      <c r="F375" t="s">
-        <v>985</v>
       </c>
       <c r="G375" t="s">
         <v>271</v>
@@ -14142,10 +14139,10 @@
     </row>
     <row r="376" spans="1:12">
       <c r="B376" s="10" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C376" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D376" t="s">
         <v>48</v>
@@ -14154,7 +14151,7 @@
         <v>49</v>
       </c>
       <c r="F376" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G376" t="s">
         <v>51</v>
@@ -14165,10 +14162,10 @@
     </row>
     <row r="377" spans="1:12">
       <c r="B377" s="10" t="s">
+        <v>986</v>
+      </c>
+      <c r="C377" t="s">
         <v>987</v>
-      </c>
-      <c r="C377" t="s">
-        <v>988</v>
       </c>
       <c r="D377" t="s">
         <v>48</v>
@@ -14177,7 +14174,7 @@
         <v>49</v>
       </c>
       <c r="F377" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="G377" t="s">
         <v>51</v>
@@ -14188,10 +14185,10 @@
     </row>
     <row r="378" spans="1:12">
       <c r="B378" s="10" t="s">
+        <v>989</v>
+      </c>
+      <c r="C378" t="s">
         <v>990</v>
-      </c>
-      <c r="C378" t="s">
-        <v>991</v>
       </c>
       <c r="D378" t="s">
         <v>48</v>
@@ -14200,7 +14197,7 @@
         <v>49</v>
       </c>
       <c r="F378" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G378" t="s">
         <v>51</v>
@@ -14211,10 +14208,10 @@
     </row>
     <row r="379" spans="1:12">
       <c r="B379" s="10" t="s">
+        <v>991</v>
+      </c>
+      <c r="C379" t="s">
         <v>992</v>
-      </c>
-      <c r="C379" t="s">
-        <v>993</v>
       </c>
       <c r="D379" t="s">
         <v>48</v>
@@ -14223,7 +14220,7 @@
         <v>49</v>
       </c>
       <c r="F379" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G379" t="s">
         <v>51</v>
@@ -14234,22 +14231,22 @@
     </row>
     <row r="380" spans="1:12">
       <c r="B380" s="10" t="s">
+        <v>993</v>
+      </c>
+      <c r="C380" t="s">
         <v>994</v>
       </c>
-      <c r="C380" t="s">
+      <c r="D380" t="s">
         <v>995</v>
       </c>
-      <c r="D380" t="s">
+      <c r="E380" t="s">
+        <v>49</v>
+      </c>
+      <c r="F380" t="s">
         <v>996</v>
       </c>
-      <c r="E380" t="s">
-        <v>49</v>
-      </c>
-      <c r="F380" t="s">
-        <v>997</v>
-      </c>
       <c r="G380" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H380" s="13" t="s">
         <v>39</v>
@@ -14257,19 +14254,19 @@
     </row>
     <row r="381" spans="1:12">
       <c r="B381" s="11" t="s">
+        <v>997</v>
+      </c>
+      <c r="C381" s="8" t="s">
         <v>998</v>
       </c>
-      <c r="C381" s="8" t="s">
+      <c r="D381" s="8" t="s">
+        <v>946</v>
+      </c>
+      <c r="E381" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F381" s="8" t="s">
         <v>999</v>
-      </c>
-      <c r="D381" s="8" t="s">
-        <v>947</v>
-      </c>
-      <c r="E381" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F381" s="8" t="s">
-        <v>1000</v>
       </c>
       <c r="G381" s="8" t="s">
         <v>271</v>
@@ -14283,10 +14280,10 @@
         <v>13</v>
       </c>
       <c r="B382" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C382" t="s">
         <v>1001</v>
-      </c>
-      <c r="C382" t="s">
-        <v>1002</v>
       </c>
       <c r="D382" t="s">
         <v>436</v>
@@ -14310,10 +14307,10 @@
         <v>57</v>
       </c>
       <c r="K382" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="L382" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="383" spans="1:12">
@@ -14341,7 +14338,7 @@
     </row>
     <row r="384" spans="1:12">
       <c r="B384" s="9" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C384" s="4" t="s">
         <v>160</v>
@@ -14353,7 +14350,7 @@
         <v>49</v>
       </c>
       <c r="F384" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G384" s="4" t="s">
         <v>102</v>
@@ -14364,10 +14361,10 @@
     </row>
     <row r="385" spans="1:12">
       <c r="B385" s="11" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C385" s="8" t="s">
         <v>1006</v>
-      </c>
-      <c r="C385" s="8" t="s">
-        <v>1007</v>
       </c>
       <c r="D385" s="8" t="s">
         <v>102</v>
@@ -14376,7 +14373,7 @@
         <v>49</v>
       </c>
       <c r="F385" s="8" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="G385" s="8" t="s">
         <v>102</v>
@@ -14390,10 +14387,10 @@
         <v>13</v>
       </c>
       <c r="B386" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C386" t="s">
         <v>1009</v>
-      </c>
-      <c r="C386" t="s">
-        <v>1010</v>
       </c>
       <c r="D386" t="s">
         <v>436</v>
@@ -14420,7 +14417,7 @@
         <v>437</v>
       </c>
       <c r="L386" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="387" spans="1:12">
@@ -14448,10 +14445,10 @@
     </row>
     <row r="388" spans="1:12">
       <c r="B388" s="9" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C388" s="4" t="s">
         <v>1011</v>
-      </c>
-      <c r="C388" s="4" t="s">
-        <v>1012</v>
       </c>
       <c r="D388" s="4" t="s">
         <v>100</v>
@@ -14460,7 +14457,7 @@
         <v>49</v>
       </c>
       <c r="F388" s="4" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="G388" s="4" t="s">
         <v>102</v>
@@ -14471,19 +14468,19 @@
     </row>
     <row r="389" spans="1:12">
       <c r="B389" s="10" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C389" t="s">
         <v>1014</v>
       </c>
-      <c r="C389" t="s">
+      <c r="D389" t="s">
         <v>1015</v>
       </c>
-      <c r="D389" t="s">
+      <c r="E389" t="s">
+        <v>49</v>
+      </c>
+      <c r="F389" t="s">
         <v>1016</v>
-      </c>
-      <c r="E389" t="s">
-        <v>49</v>
-      </c>
-      <c r="F389" t="s">
-        <v>1017</v>
       </c>
       <c r="G389" t="s">
         <v>234</v>
@@ -14494,19 +14491,19 @@
     </row>
     <row r="390" spans="1:12">
       <c r="B390" s="10" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C390" t="s">
         <v>1018</v>
       </c>
-      <c r="C390" t="s">
+      <c r="D390" t="s">
         <v>1019</v>
       </c>
-      <c r="D390" t="s">
+      <c r="E390" t="s">
+        <v>49</v>
+      </c>
+      <c r="F390" t="s">
         <v>1020</v>
-      </c>
-      <c r="E390" t="s">
-        <v>49</v>
-      </c>
-      <c r="F390" t="s">
-        <v>1021</v>
       </c>
       <c r="G390" t="s">
         <v>234</v>
@@ -14517,10 +14514,10 @@
     </row>
     <row r="391" spans="1:12">
       <c r="B391" s="10" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C391" t="s">
         <v>1022</v>
-      </c>
-      <c r="C391" t="s">
-        <v>1023</v>
       </c>
       <c r="D391" t="s">
         <v>120</v>
@@ -14529,7 +14526,7 @@
         <v>49</v>
       </c>
       <c r="F391" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="G391" t="s">
         <v>120</v>
@@ -14540,19 +14537,19 @@
     </row>
     <row r="392" spans="1:12">
       <c r="B392" s="10" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C392" t="s">
         <v>1025</v>
       </c>
-      <c r="C392" t="s">
+      <c r="D392" t="s">
         <v>1026</v>
       </c>
-      <c r="D392" t="s">
+      <c r="E392" t="s">
+        <v>49</v>
+      </c>
+      <c r="F392" t="s">
         <v>1027</v>
-      </c>
-      <c r="E392" t="s">
-        <v>49</v>
-      </c>
-      <c r="F392" t="s">
-        <v>1028</v>
       </c>
       <c r="G392" t="s">
         <v>234</v>
@@ -14563,10 +14560,10 @@
     </row>
     <row r="393" spans="1:12">
       <c r="B393" s="10" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C393" t="s">
         <v>1029</v>
-      </c>
-      <c r="C393" t="s">
-        <v>1030</v>
       </c>
       <c r="D393" t="s">
         <v>120</v>
@@ -14575,7 +14572,7 @@
         <v>49</v>
       </c>
       <c r="F393" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="G393" t="s">
         <v>120</v>
@@ -14586,19 +14583,19 @@
     </row>
     <row r="394" spans="1:12">
       <c r="B394" s="10" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C394" t="s">
         <v>1032</v>
       </c>
-      <c r="C394" t="s">
+      <c r="D394" t="s">
         <v>1033</v>
       </c>
-      <c r="D394" t="s">
+      <c r="E394" t="s">
+        <v>49</v>
+      </c>
+      <c r="F394" t="s">
         <v>1034</v>
-      </c>
-      <c r="E394" t="s">
-        <v>49</v>
-      </c>
-      <c r="F394" t="s">
-        <v>1035</v>
       </c>
       <c r="G394" t="s">
         <v>100</v>
@@ -14609,19 +14606,19 @@
     </row>
     <row r="395" spans="1:12">
       <c r="B395" s="10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C395" t="s">
         <v>1036</v>
       </c>
-      <c r="C395" t="s">
+      <c r="D395" t="s">
         <v>1037</v>
       </c>
-      <c r="D395" t="s">
+      <c r="E395" t="s">
+        <v>49</v>
+      </c>
+      <c r="F395" t="s">
         <v>1038</v>
-      </c>
-      <c r="E395" t="s">
-        <v>49</v>
-      </c>
-      <c r="F395" t="s">
-        <v>1039</v>
       </c>
       <c r="G395" t="s">
         <v>100</v>
@@ -14632,19 +14629,19 @@
     </row>
     <row r="396" spans="1:12">
       <c r="B396" s="10" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C396" t="s">
         <v>1040</v>
       </c>
-      <c r="C396" t="s">
+      <c r="D396" t="s">
         <v>1041</v>
       </c>
-      <c r="D396" t="s">
+      <c r="E396" t="s">
+        <v>49</v>
+      </c>
+      <c r="F396" t="s">
         <v>1042</v>
-      </c>
-      <c r="E396" t="s">
-        <v>49</v>
-      </c>
-      <c r="F396" t="s">
-        <v>1043</v>
       </c>
       <c r="G396" t="s">
         <v>100</v>
@@ -14655,19 +14652,19 @@
     </row>
     <row r="397" spans="1:12">
       <c r="B397" s="11" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C397" s="8" t="s">
         <v>1044</v>
       </c>
-      <c r="C397" s="8" t="s">
+      <c r="D397" s="8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E397" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F397" s="8" t="s">
         <v>1045</v>
-      </c>
-      <c r="D397" s="8" t="s">
-        <v>1034</v>
-      </c>
-      <c r="E397" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F397" s="8" t="s">
-        <v>1046</v>
       </c>
       <c r="G397" s="8" t="s">
         <v>100</v>
@@ -14681,10 +14678,10 @@
         <v>13</v>
       </c>
       <c r="B398" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C398" t="s">
         <v>1047</v>
-      </c>
-      <c r="C398" t="s">
-        <v>1048</v>
       </c>
       <c r="D398" t="s">
         <v>436</v>
@@ -14708,10 +14705,10 @@
         <v>39</v>
       </c>
       <c r="K398" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="L398" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="399" spans="1:12">
@@ -14739,10 +14736,10 @@
     </row>
     <row r="400" spans="1:12">
       <c r="B400" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C400" s="4" t="s">
         <v>1050</v>
-      </c>
-      <c r="C400" s="4" t="s">
-        <v>1051</v>
       </c>
       <c r="D400" s="4" t="s">
         <v>471</v>
@@ -14751,7 +14748,7 @@
         <v>49</v>
       </c>
       <c r="F400" s="4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="G400" s="4" t="s">
         <v>473</v>
@@ -14762,19 +14759,19 @@
     </row>
     <row r="401" spans="1:12">
       <c r="B401" s="10" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C401" t="s">
         <v>1053</v>
       </c>
-      <c r="C401" t="s">
+      <c r="D401" t="s">
         <v>1054</v>
       </c>
-      <c r="D401" t="s">
+      <c r="E401" t="s">
+        <v>49</v>
+      </c>
+      <c r="F401" t="s">
         <v>1055</v>
-      </c>
-      <c r="E401" t="s">
-        <v>49</v>
-      </c>
-      <c r="F401" t="s">
-        <v>1056</v>
       </c>
       <c r="G401" t="s">
         <v>473</v>
@@ -14785,19 +14782,19 @@
     </row>
     <row r="402" spans="1:12">
       <c r="B402" s="10" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C402" t="s">
         <v>1057</v>
       </c>
-      <c r="C402" t="s">
+      <c r="D402" t="s">
         <v>1058</v>
       </c>
-      <c r="D402" t="s">
+      <c r="E402" t="s">
+        <v>49</v>
+      </c>
+      <c r="F402" t="s">
         <v>1059</v>
-      </c>
-      <c r="E402" t="s">
-        <v>49</v>
-      </c>
-      <c r="F402" t="s">
-        <v>1060</v>
       </c>
       <c r="G402" t="s">
         <v>473</v>
@@ -14808,10 +14805,10 @@
     </row>
     <row r="403" spans="1:12">
       <c r="B403" s="11" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C403" s="8" t="s">
         <v>1061</v>
-      </c>
-      <c r="C403" s="8" t="s">
-        <v>1062</v>
       </c>
       <c r="D403" s="8" t="s">
         <v>473</v>
@@ -14820,7 +14817,7 @@
         <v>49</v>
       </c>
       <c r="F403" s="8" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G403" s="8" t="s">
         <v>473</v>
@@ -14834,10 +14831,10 @@
         <v>13</v>
       </c>
       <c r="B404" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C404" t="s">
         <v>1064</v>
-      </c>
-      <c r="C404" t="s">
-        <v>1065</v>
       </c>
       <c r="D404" t="s">
         <v>436</v>
@@ -14864,7 +14861,7 @@
         <v>437</v>
       </c>
       <c r="L404" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="405" spans="1:12">
@@ -14892,19 +14889,19 @@
     </row>
     <row r="406" spans="1:12">
       <c r="B406" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C406" s="4" t="s">
         <v>1066</v>
       </c>
-      <c r="C406" s="4" t="s">
+      <c r="D406" s="4" t="s">
         <v>1067</v>
       </c>
-      <c r="D406" s="4" t="s">
+      <c r="E406" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F406" s="4" t="s">
         <v>1068</v>
-      </c>
-      <c r="E406" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F406" s="4" t="s">
-        <v>1069</v>
       </c>
       <c r="G406" s="4" t="s">
         <v>94</v>
@@ -14915,19 +14912,19 @@
     </row>
     <row r="407" spans="1:12">
       <c r="B407" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C407" t="s">
         <v>1070</v>
       </c>
-      <c r="C407" t="s">
-        <v>1071</v>
-      </c>
       <c r="D407" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E407" t="s">
+        <v>49</v>
+      </c>
+      <c r="F407" t="s">
         <v>1068</v>
-      </c>
-      <c r="E407" t="s">
-        <v>49</v>
-      </c>
-      <c r="F407" t="s">
-        <v>1069</v>
       </c>
       <c r="G407" t="s">
         <v>94</v>
@@ -14938,10 +14935,10 @@
     </row>
     <row r="408" spans="1:12">
       <c r="B408" s="10" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C408" t="s">
         <v>1072</v>
-      </c>
-      <c r="C408" t="s">
-        <v>1073</v>
       </c>
       <c r="D408" t="s">
         <v>362</v>
@@ -14950,7 +14947,7 @@
         <v>49</v>
       </c>
       <c r="F408" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G408" t="s">
         <v>362</v>
@@ -14961,19 +14958,19 @@
     </row>
     <row r="409" spans="1:12">
       <c r="B409" s="10" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C409" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D409" t="s">
         <v>1067</v>
       </c>
-      <c r="D409" t="s">
+      <c r="E409" t="s">
+        <v>49</v>
+      </c>
+      <c r="F409" t="s">
         <v>1068</v>
-      </c>
-      <c r="E409" t="s">
-        <v>49</v>
-      </c>
-      <c r="F409" t="s">
-        <v>1069</v>
       </c>
       <c r="G409" t="s">
         <v>94</v>
@@ -14984,10 +14981,10 @@
     </row>
     <row r="410" spans="1:12">
       <c r="B410" s="10" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C410" t="s">
         <v>1076</v>
-      </c>
-      <c r="C410" t="s">
-        <v>1077</v>
       </c>
       <c r="D410" t="s">
         <v>341</v>
@@ -14996,7 +14993,7 @@
         <v>49</v>
       </c>
       <c r="F410" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G410" t="s">
         <v>341</v>
@@ -15007,19 +15004,19 @@
     </row>
     <row r="411" spans="1:12">
       <c r="B411" s="10" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C411" t="s">
         <v>1079</v>
       </c>
-      <c r="C411" t="s">
+      <c r="D411" t="s">
         <v>1080</v>
       </c>
-      <c r="D411" t="s">
+      <c r="E411" t="s">
+        <v>49</v>
+      </c>
+      <c r="F411" t="s">
         <v>1081</v>
-      </c>
-      <c r="E411" t="s">
-        <v>49</v>
-      </c>
-      <c r="F411" t="s">
-        <v>1082</v>
       </c>
       <c r="G411" t="s">
         <v>94</v>
@@ -15030,19 +15027,19 @@
     </row>
     <row r="412" spans="1:12">
       <c r="B412" s="10" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C412" t="s">
         <v>1083</v>
       </c>
-      <c r="C412" t="s">
+      <c r="D412" t="s">
         <v>1084</v>
       </c>
-      <c r="D412" t="s">
+      <c r="E412" t="s">
+        <v>49</v>
+      </c>
+      <c r="F412" t="s">
         <v>1085</v>
-      </c>
-      <c r="E412" t="s">
-        <v>49</v>
-      </c>
-      <c r="F412" t="s">
-        <v>1086</v>
       </c>
       <c r="G412" t="s">
         <v>341</v>
@@ -15053,19 +15050,19 @@
     </row>
     <row r="413" spans="1:12">
       <c r="B413" s="10" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C413" t="s">
         <v>1087</v>
       </c>
-      <c r="C413" t="s">
+      <c r="D413" t="s">
         <v>1088</v>
       </c>
-      <c r="D413" t="s">
+      <c r="E413" t="s">
+        <v>49</v>
+      </c>
+      <c r="F413" t="s">
         <v>1089</v>
-      </c>
-      <c r="E413" t="s">
-        <v>49</v>
-      </c>
-      <c r="F413" t="s">
-        <v>1090</v>
       </c>
       <c r="G413" t="s">
         <v>362</v>
@@ -15076,10 +15073,10 @@
     </row>
     <row r="414" spans="1:12">
       <c r="B414" s="10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C414" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D414" t="s">
         <v>362</v>
@@ -15088,7 +15085,7 @@
         <v>49</v>
       </c>
       <c r="F414" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G414" t="s">
         <v>362</v>
@@ -15099,19 +15096,19 @@
     </row>
     <row r="415" spans="1:12">
       <c r="B415" s="10" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C415" t="s">
         <v>1092</v>
       </c>
-      <c r="C415" t="s">
+      <c r="D415" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E415" t="s">
+        <v>49</v>
+      </c>
+      <c r="F415" t="s">
         <v>1093</v>
-      </c>
-      <c r="D415" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E415" t="s">
-        <v>49</v>
-      </c>
-      <c r="F415" t="s">
-        <v>1094</v>
       </c>
       <c r="G415" t="s">
         <v>94</v>
@@ -15122,19 +15119,19 @@
     </row>
     <row r="416" spans="1:12">
       <c r="B416" s="10" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C416" t="s">
         <v>1095</v>
       </c>
-      <c r="C416" t="s">
+      <c r="D416" t="s">
         <v>1096</v>
       </c>
-      <c r="D416" t="s">
+      <c r="E416" t="s">
+        <v>49</v>
+      </c>
+      <c r="F416" t="s">
         <v>1097</v>
-      </c>
-      <c r="E416" t="s">
-        <v>49</v>
-      </c>
-      <c r="F416" t="s">
-        <v>1098</v>
       </c>
       <c r="G416" t="s">
         <v>341</v>
@@ -15145,19 +15142,19 @@
     </row>
     <row r="417" spans="1:12">
       <c r="B417" s="10" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C417" t="s">
         <v>1099</v>
       </c>
-      <c r="C417" t="s">
+      <c r="D417" t="s">
         <v>1100</v>
       </c>
-      <c r="D417" t="s">
+      <c r="E417" t="s">
+        <v>49</v>
+      </c>
+      <c r="F417" t="s">
         <v>1101</v>
-      </c>
-      <c r="E417" t="s">
-        <v>49</v>
-      </c>
-      <c r="F417" t="s">
-        <v>1102</v>
       </c>
       <c r="G417" t="s">
         <v>341</v>
@@ -15168,19 +15165,19 @@
     </row>
     <row r="418" spans="1:12">
       <c r="B418" s="10" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C418" t="s">
         <v>1103</v>
       </c>
-      <c r="C418" t="s">
+      <c r="D418" t="s">
         <v>1104</v>
       </c>
-      <c r="D418" t="s">
+      <c r="E418" t="s">
+        <v>49</v>
+      </c>
+      <c r="F418" t="s">
         <v>1105</v>
-      </c>
-      <c r="E418" t="s">
-        <v>49</v>
-      </c>
-      <c r="F418" t="s">
-        <v>1106</v>
       </c>
       <c r="G418" t="s">
         <v>341</v>
@@ -15191,19 +15188,19 @@
     </row>
     <row r="419" spans="1:12">
       <c r="B419" s="10" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C419" t="s">
         <v>1107</v>
       </c>
-      <c r="C419" t="s">
+      <c r="D419" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E419" t="s">
+        <v>49</v>
+      </c>
+      <c r="F419" t="s">
         <v>1108</v>
-      </c>
-      <c r="D419" t="s">
-        <v>1105</v>
-      </c>
-      <c r="E419" t="s">
-        <v>49</v>
-      </c>
-      <c r="F419" t="s">
-        <v>1109</v>
       </c>
       <c r="G419" t="s">
         <v>341</v>
@@ -15214,10 +15211,10 @@
     </row>
     <row r="420" spans="1:12">
       <c r="B420" s="10" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C420" t="s">
         <v>1110</v>
-      </c>
-      <c r="C420" t="s">
-        <v>1111</v>
       </c>
       <c r="D420" t="s">
         <v>341</v>
@@ -15226,7 +15223,7 @@
         <v>49</v>
       </c>
       <c r="F420" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="G420" t="s">
         <v>341</v>
@@ -15237,10 +15234,10 @@
     </row>
     <row r="421" spans="1:12">
       <c r="B421" s="10" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C421" t="s">
         <v>1113</v>
-      </c>
-      <c r="C421" t="s">
-        <v>1114</v>
       </c>
       <c r="D421" t="s">
         <v>92</v>
@@ -15249,7 +15246,7 @@
         <v>49</v>
       </c>
       <c r="F421" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="G421" t="s">
         <v>94</v>
@@ -15260,10 +15257,10 @@
     </row>
     <row r="422" spans="1:12">
       <c r="B422" s="10" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C422" t="s">
         <v>1116</v>
-      </c>
-      <c r="C422" t="s">
-        <v>1117</v>
       </c>
       <c r="D422" t="s">
         <v>92</v>
@@ -15272,7 +15269,7 @@
         <v>49</v>
       </c>
       <c r="F422" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="G422" t="s">
         <v>94</v>
@@ -15283,10 +15280,10 @@
     </row>
     <row r="423" spans="1:12">
       <c r="B423" s="10" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C423" t="s">
         <v>1119</v>
-      </c>
-      <c r="C423" t="s">
-        <v>1120</v>
       </c>
       <c r="D423" t="s">
         <v>92</v>
@@ -15295,7 +15292,7 @@
         <v>49</v>
       </c>
       <c r="F423" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G423" t="s">
         <v>94</v>
@@ -15306,19 +15303,19 @@
     </row>
     <row r="424" spans="1:12">
       <c r="B424" s="10" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C424" t="s">
         <v>1122</v>
       </c>
-      <c r="C424" t="s">
+      <c r="D424" t="s">
         <v>1123</v>
       </c>
-      <c r="D424" t="s">
+      <c r="E424" t="s">
+        <v>49</v>
+      </c>
+      <c r="F424" t="s">
         <v>1124</v>
-      </c>
-      <c r="E424" t="s">
-        <v>49</v>
-      </c>
-      <c r="F424" t="s">
-        <v>1125</v>
       </c>
       <c r="G424" t="s">
         <v>341</v>
@@ -15329,19 +15326,19 @@
     </row>
     <row r="425" spans="1:12">
       <c r="B425" s="10" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C425" t="s">
         <v>1126</v>
       </c>
-      <c r="C425" t="s">
+      <c r="D425" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E425" t="s">
+        <v>49</v>
+      </c>
+      <c r="F425" t="s">
         <v>1127</v>
-      </c>
-      <c r="D425" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E425" t="s">
-        <v>49</v>
-      </c>
-      <c r="F425" t="s">
-        <v>1128</v>
       </c>
       <c r="G425" t="s">
         <v>341</v>
@@ -15352,19 +15349,19 @@
     </row>
     <row r="426" spans="1:12">
       <c r="B426" s="10" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C426" t="s">
         <v>1129</v>
       </c>
-      <c r="C426" t="s">
+      <c r="D426" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E426" t="s">
+        <v>49</v>
+      </c>
+      <c r="F426" t="s">
         <v>1130</v>
-      </c>
-      <c r="D426" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E426" t="s">
-        <v>49</v>
-      </c>
-      <c r="F426" t="s">
-        <v>1131</v>
       </c>
       <c r="G426" t="s">
         <v>341</v>
@@ -15375,19 +15372,19 @@
     </row>
     <row r="427" spans="1:12">
       <c r="B427" s="11" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C427" s="8" t="s">
         <v>1132</v>
       </c>
-      <c r="C427" s="8" t="s">
+      <c r="D427" s="8" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E427" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F427" s="8" t="s">
         <v>1133</v>
-      </c>
-      <c r="D427" s="8" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E427" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F427" s="8" t="s">
-        <v>1134</v>
       </c>
       <c r="G427" s="8" t="s">
         <v>341</v>
@@ -15401,10 +15398,10 @@
         <v>13</v>
       </c>
       <c r="B428" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C428" t="s">
         <v>1135</v>
-      </c>
-      <c r="C428" t="s">
-        <v>1136</v>
       </c>
       <c r="D428" t="s">
         <v>436</v>
@@ -15431,7 +15428,7 @@
         <v>437</v>
       </c>
       <c r="L428" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="429" spans="1:12">
@@ -15459,10 +15456,10 @@
     </row>
     <row r="430" spans="1:12">
       <c r="B430" s="9" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C430" s="4" t="s">
         <v>1137</v>
-      </c>
-      <c r="C430" s="4" t="s">
-        <v>1138</v>
       </c>
       <c r="D430" s="4" t="s">
         <v>471</v>
@@ -15471,7 +15468,7 @@
         <v>49</v>
       </c>
       <c r="F430" s="4" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G430" s="4" t="s">
         <v>473</v>
@@ -15482,10 +15479,10 @@
     </row>
     <row r="431" spans="1:12">
       <c r="B431" s="10" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C431" t="s">
         <v>1140</v>
-      </c>
-      <c r="C431" t="s">
-        <v>1141</v>
       </c>
       <c r="D431" t="s">
         <v>471</v>
@@ -15494,7 +15491,7 @@
         <v>49</v>
       </c>
       <c r="F431" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="G431" t="s">
         <v>473</v>
@@ -15505,10 +15502,10 @@
     </row>
     <row r="432" spans="1:12">
       <c r="B432" s="10" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C432" t="s">
         <v>1143</v>
-      </c>
-      <c r="C432" t="s">
-        <v>1144</v>
       </c>
       <c r="D432" t="s">
         <v>471</v>
@@ -15517,7 +15514,7 @@
         <v>49</v>
       </c>
       <c r="F432" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G432" t="s">
         <v>473</v>
@@ -15528,10 +15525,10 @@
     </row>
     <row r="433" spans="1:12">
       <c r="B433" s="10" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C433" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="D433" t="s">
         <v>471</v>
@@ -15540,7 +15537,7 @@
         <v>49</v>
       </c>
       <c r="F433" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G433" t="s">
         <v>473</v>
@@ -15551,10 +15548,10 @@
     </row>
     <row r="434" spans="1:12">
       <c r="B434" s="10" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C434" t="s">
         <v>1148</v>
-      </c>
-      <c r="C434" t="s">
-        <v>1149</v>
       </c>
       <c r="D434" t="s">
         <v>216</v>
@@ -15563,7 +15560,7 @@
         <v>49</v>
       </c>
       <c r="F434" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G434" t="s">
         <v>216</v>
@@ -15574,10 +15571,10 @@
     </row>
     <row r="435" spans="1:12">
       <c r="B435" s="10" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C435" t="s">
         <v>1151</v>
-      </c>
-      <c r="C435" t="s">
-        <v>1152</v>
       </c>
       <c r="D435" t="s">
         <v>216</v>
@@ -15586,7 +15583,7 @@
         <v>49</v>
       </c>
       <c r="F435" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G435" t="s">
         <v>216</v>
@@ -15597,10 +15594,10 @@
     </row>
     <row r="436" spans="1:12">
       <c r="B436" s="10" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C436" t="s">
         <v>1154</v>
-      </c>
-      <c r="C436" t="s">
-        <v>1155</v>
       </c>
       <c r="D436" t="s">
         <v>471</v>
@@ -15609,7 +15606,7 @@
         <v>49</v>
       </c>
       <c r="F436" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="G436" t="s">
         <v>473</v>
@@ -15620,10 +15617,10 @@
     </row>
     <row r="437" spans="1:12">
       <c r="B437" s="10" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C437" t="s">
         <v>1157</v>
-      </c>
-      <c r="C437" t="s">
-        <v>1158</v>
       </c>
       <c r="D437" t="s">
         <v>216</v>
@@ -15632,7 +15629,7 @@
         <v>49</v>
       </c>
       <c r="F437" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="G437" t="s">
         <v>216</v>
@@ -15643,10 +15640,10 @@
     </row>
     <row r="438" spans="1:12">
       <c r="B438" s="10" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C438" t="s">
         <v>1160</v>
-      </c>
-      <c r="C438" t="s">
-        <v>1161</v>
       </c>
       <c r="D438" t="s">
         <v>471</v>
@@ -15655,7 +15652,7 @@
         <v>49</v>
       </c>
       <c r="F438" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="G438" t="s">
         <v>473</v>
@@ -15666,10 +15663,10 @@
     </row>
     <row r="439" spans="1:12">
       <c r="B439" s="11" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C439" s="8" t="s">
         <v>1163</v>
-      </c>
-      <c r="C439" s="8" t="s">
-        <v>1164</v>
       </c>
       <c r="D439" s="8" t="s">
         <v>471</v>
@@ -15678,7 +15675,7 @@
         <v>49</v>
       </c>
       <c r="F439" s="8" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="G439" s="8" t="s">
         <v>473</v>
@@ -15692,10 +15689,10 @@
         <v>13</v>
       </c>
       <c r="B440" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C440" t="s">
         <v>1166</v>
-      </c>
-      <c r="C440" t="s">
-        <v>1167</v>
       </c>
       <c r="D440" t="s">
         <v>436</v>
@@ -15704,7 +15701,7 @@
         <v>17</v>
       </c>
       <c r="F440" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G440" t="s">
         <v>160</v>
@@ -15722,7 +15719,7 @@
         <v>437</v>
       </c>
       <c r="L440" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="441" spans="1:12">
@@ -15750,19 +15747,19 @@
     </row>
     <row r="442" spans="1:12">
       <c r="B442" s="9" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C442" s="4" t="s">
         <v>1169</v>
       </c>
-      <c r="C442" s="4" t="s">
+      <c r="D442" s="4" t="s">
         <v>1170</v>
       </c>
-      <c r="D442" s="4" t="s">
+      <c r="E442" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F442" s="4" t="s">
         <v>1171</v>
-      </c>
-      <c r="E442" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F442" s="4" t="s">
-        <v>1172</v>
       </c>
       <c r="G442" s="4" t="s">
         <v>389</v>
@@ -15773,19 +15770,19 @@
     </row>
     <row r="443" spans="1:12">
       <c r="B443" s="10" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C443" t="s">
         <v>1173</v>
       </c>
-      <c r="C443" t="s">
+      <c r="D443" t="s">
         <v>1174</v>
       </c>
-      <c r="D443" t="s">
+      <c r="E443" t="s">
+        <v>49</v>
+      </c>
+      <c r="F443" t="s">
         <v>1175</v>
-      </c>
-      <c r="E443" t="s">
-        <v>49</v>
-      </c>
-      <c r="F443" t="s">
-        <v>1176</v>
       </c>
       <c r="G443" t="s">
         <v>391</v>
@@ -15796,19 +15793,19 @@
     </row>
     <row r="444" spans="1:12">
       <c r="B444" s="10" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C444" t="s">
         <v>1177</v>
       </c>
-      <c r="C444" t="s">
+      <c r="D444" t="s">
         <v>1178</v>
       </c>
-      <c r="D444" t="s">
+      <c r="E444" t="s">
+        <v>49</v>
+      </c>
+      <c r="F444" t="s">
         <v>1179</v>
-      </c>
-      <c r="E444" t="s">
-        <v>49</v>
-      </c>
-      <c r="F444" t="s">
-        <v>1180</v>
       </c>
       <c r="G444" t="s">
         <v>181</v>
@@ -15819,19 +15816,19 @@
     </row>
     <row r="445" spans="1:12">
       <c r="B445" s="10" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C445" t="s">
         <v>1181</v>
       </c>
-      <c r="C445" t="s">
+      <c r="D445" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E445" t="s">
+        <v>49</v>
+      </c>
+      <c r="F445" t="s">
         <v>1182</v>
-      </c>
-      <c r="D445" t="s">
-        <v>1179</v>
-      </c>
-      <c r="E445" t="s">
-        <v>49</v>
-      </c>
-      <c r="F445" t="s">
-        <v>1183</v>
       </c>
       <c r="G445" t="s">
         <v>181</v>
@@ -15842,19 +15839,19 @@
     </row>
     <row r="446" spans="1:12">
       <c r="B446" s="10" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C446" t="s">
         <v>1184</v>
       </c>
-      <c r="C446" t="s">
+      <c r="D446" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E446" t="s">
+        <v>49</v>
+      </c>
+      <c r="F446" t="s">
         <v>1185</v>
-      </c>
-      <c r="D446" t="s">
-        <v>1179</v>
-      </c>
-      <c r="E446" t="s">
-        <v>49</v>
-      </c>
-      <c r="F446" t="s">
-        <v>1186</v>
       </c>
       <c r="G446" t="s">
         <v>181</v>
@@ -15865,19 +15862,19 @@
     </row>
     <row r="447" spans="1:12">
       <c r="B447" s="10" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C447" t="s">
         <v>1187</v>
       </c>
-      <c r="C447" t="s">
+      <c r="D447" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E447" t="s">
+        <v>49</v>
+      </c>
+      <c r="F447" t="s">
         <v>1188</v>
-      </c>
-      <c r="D447" t="s">
-        <v>1179</v>
-      </c>
-      <c r="E447" t="s">
-        <v>49</v>
-      </c>
-      <c r="F447" t="s">
-        <v>1189</v>
       </c>
       <c r="G447" t="s">
         <v>181</v>
@@ -15888,19 +15885,19 @@
     </row>
     <row r="448" spans="1:12">
       <c r="B448" s="10" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C448" t="s">
         <v>1190</v>
       </c>
-      <c r="C448" t="s">
+      <c r="D448" t="s">
         <v>1191</v>
       </c>
-      <c r="D448" t="s">
+      <c r="E448" t="s">
+        <v>49</v>
+      </c>
+      <c r="F448" t="s">
         <v>1192</v>
-      </c>
-      <c r="E448" t="s">
-        <v>49</v>
-      </c>
-      <c r="F448" t="s">
-        <v>1193</v>
       </c>
       <c r="G448" t="s">
         <v>391</v>
@@ -15911,10 +15908,10 @@
     </row>
     <row r="449" spans="1:12">
       <c r="B449" s="10" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C449" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="D449" t="s">
         <v>391</v>
@@ -15923,7 +15920,7 @@
         <v>49</v>
       </c>
       <c r="F449" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="G449" t="s">
         <v>391</v>
@@ -15934,10 +15931,10 @@
     </row>
     <row r="450" spans="1:12">
       <c r="B450" s="10" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C450" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="D450" t="s">
         <v>391</v>
@@ -15946,7 +15943,7 @@
         <v>49</v>
       </c>
       <c r="F450" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="G450" t="s">
         <v>391</v>
@@ -15957,10 +15954,10 @@
     </row>
     <row r="451" spans="1:12">
       <c r="B451" s="10" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C451" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="D451" t="s">
         <v>391</v>
@@ -15969,7 +15966,7 @@
         <v>49</v>
       </c>
       <c r="F451" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="G451" t="s">
         <v>391</v>
@@ -15980,19 +15977,19 @@
     </row>
     <row r="452" spans="1:12">
       <c r="B452" s="10" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C452" t="s">
         <v>1198</v>
       </c>
-      <c r="C452" t="s">
+      <c r="D452" t="s">
         <v>1199</v>
       </c>
-      <c r="D452" t="s">
+      <c r="E452" t="s">
+        <v>49</v>
+      </c>
+      <c r="F452" t="s">
         <v>1200</v>
-      </c>
-      <c r="E452" t="s">
-        <v>49</v>
-      </c>
-      <c r="F452" t="s">
-        <v>1201</v>
       </c>
       <c r="G452" t="s">
         <v>391</v>
@@ -16003,10 +16000,10 @@
     </row>
     <row r="453" spans="1:12">
       <c r="B453" s="10" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C453" t="s">
         <v>1202</v>
-      </c>
-      <c r="C453" t="s">
-        <v>1203</v>
       </c>
       <c r="D453" t="s">
         <v>391</v>
@@ -16015,7 +16012,7 @@
         <v>49</v>
       </c>
       <c r="F453" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="G453" t="s">
         <v>391</v>
@@ -16026,19 +16023,19 @@
     </row>
     <row r="454" spans="1:12">
       <c r="B454" s="10" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C454" t="s">
         <v>1205</v>
       </c>
-      <c r="C454" t="s">
+      <c r="D454" t="s">
         <v>1206</v>
       </c>
-      <c r="D454" t="s">
+      <c r="E454" t="s">
+        <v>49</v>
+      </c>
+      <c r="F454" t="s">
         <v>1207</v>
-      </c>
-      <c r="E454" t="s">
-        <v>49</v>
-      </c>
-      <c r="F454" t="s">
-        <v>1208</v>
       </c>
       <c r="G454" t="s">
         <v>389</v>
@@ -16049,19 +16046,19 @@
     </row>
     <row r="455" spans="1:12">
       <c r="B455" s="10" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C455" t="s">
         <v>1209</v>
       </c>
-      <c r="C455" t="s">
+      <c r="D455" t="s">
         <v>1210</v>
       </c>
-      <c r="D455" t="s">
+      <c r="E455" t="s">
+        <v>49</v>
+      </c>
+      <c r="F455" t="s">
         <v>1211</v>
-      </c>
-      <c r="E455" t="s">
-        <v>49</v>
-      </c>
-      <c r="F455" t="s">
-        <v>1212</v>
       </c>
       <c r="G455" t="s">
         <v>71</v>
@@ -16072,19 +16069,19 @@
     </row>
     <row r="456" spans="1:12">
       <c r="B456" s="10" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C456" t="s">
         <v>1213</v>
       </c>
-      <c r="C456" t="s">
+      <c r="D456" t="s">
         <v>1214</v>
       </c>
-      <c r="D456" t="s">
+      <c r="E456" t="s">
+        <v>49</v>
+      </c>
+      <c r="F456" t="s">
         <v>1215</v>
-      </c>
-      <c r="E456" t="s">
-        <v>49</v>
-      </c>
-      <c r="F456" t="s">
-        <v>1216</v>
       </c>
       <c r="G456" t="s">
         <v>389</v>
@@ -16095,19 +16092,19 @@
     </row>
     <row r="457" spans="1:12">
       <c r="B457" s="11" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C457" s="8" t="s">
         <v>1217</v>
       </c>
-      <c r="C457" s="8" t="s">
-        <v>1218</v>
-      </c>
       <c r="D457" s="8" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E457" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F457" s="8" t="s">
         <v>1171</v>
-      </c>
-      <c r="E457" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F457" s="8" t="s">
-        <v>1172</v>
       </c>
       <c r="G457" s="8" t="s">
         <v>389</v>
@@ -16121,10 +16118,10 @@
         <v>13</v>
       </c>
       <c r="B458" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C458" t="s">
         <v>1219</v>
-      </c>
-      <c r="C458" t="s">
-        <v>1220</v>
       </c>
       <c r="D458" t="s">
         <v>436</v>
@@ -16151,7 +16148,7 @@
         <v>437</v>
       </c>
       <c r="L458" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="459" spans="1:12">
@@ -16179,10 +16176,10 @@
     </row>
     <row r="460" spans="1:12">
       <c r="B460" s="9" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C460" s="4" t="s">
         <v>1221</v>
-      </c>
-      <c r="C460" s="4" t="s">
-        <v>1222</v>
       </c>
       <c r="D460" s="4" t="s">
         <v>196</v>
@@ -16191,7 +16188,7 @@
         <v>49</v>
       </c>
       <c r="F460" s="4" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="G460" s="4" t="s">
         <v>196</v>
@@ -16202,10 +16199,10 @@
     </row>
     <row r="461" spans="1:12">
       <c r="B461" s="10" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C461" t="s">
         <v>1224</v>
-      </c>
-      <c r="C461" t="s">
-        <v>1225</v>
       </c>
       <c r="D461" t="s">
         <v>181</v>
@@ -16214,7 +16211,7 @@
         <v>49</v>
       </c>
       <c r="F461" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="G461" t="s">
         <v>181</v>
@@ -16225,10 +16222,10 @@
     </row>
     <row r="462" spans="1:12">
       <c r="B462" s="10" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C462" t="s">
         <v>1227</v>
-      </c>
-      <c r="C462" t="s">
-        <v>1228</v>
       </c>
       <c r="D462" t="s">
         <v>317</v>
@@ -16237,7 +16234,7 @@
         <v>49</v>
       </c>
       <c r="F462" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="G462" t="s">
         <v>317</v>
@@ -16248,10 +16245,10 @@
     </row>
     <row r="463" spans="1:12">
       <c r="B463" s="10" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C463" t="s">
         <v>1230</v>
-      </c>
-      <c r="C463" t="s">
-        <v>1231</v>
       </c>
       <c r="D463" t="s">
         <v>317</v>
@@ -16260,7 +16257,7 @@
         <v>49</v>
       </c>
       <c r="F463" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="G463" t="s">
         <v>317</v>
@@ -16271,19 +16268,19 @@
     </row>
     <row r="464" spans="1:12">
       <c r="B464" s="10" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C464" t="s">
         <v>1233</v>
       </c>
-      <c r="C464" t="s">
+      <c r="D464" t="s">
         <v>1234</v>
       </c>
-      <c r="D464" t="s">
+      <c r="E464" t="s">
+        <v>49</v>
+      </c>
+      <c r="F464" t="s">
         <v>1235</v>
-      </c>
-      <c r="E464" t="s">
-        <v>49</v>
-      </c>
-      <c r="F464" t="s">
-        <v>1236</v>
       </c>
       <c r="G464" t="s">
         <v>317</v>
@@ -16294,10 +16291,10 @@
     </row>
     <row r="465" spans="1:12">
       <c r="B465" s="10" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C465" t="s">
         <v>1237</v>
-      </c>
-      <c r="C465" t="s">
-        <v>1238</v>
       </c>
       <c r="D465" t="s">
         <v>317</v>
@@ -16306,7 +16303,7 @@
         <v>49</v>
       </c>
       <c r="F465" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="G465" t="s">
         <v>317</v>
@@ -16317,10 +16314,10 @@
     </row>
     <row r="466" spans="1:12">
       <c r="B466" s="10" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C466" t="s">
         <v>1240</v>
-      </c>
-      <c r="C466" t="s">
-        <v>1241</v>
       </c>
       <c r="D466" t="s">
         <v>317</v>
@@ -16329,7 +16326,7 @@
         <v>49</v>
       </c>
       <c r="F466" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="G466" t="s">
         <v>317</v>
@@ -16340,19 +16337,19 @@
     </row>
     <row r="467" spans="1:12">
       <c r="B467" s="10" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C467" t="s">
         <v>1243</v>
       </c>
-      <c r="C467" t="s">
+      <c r="D467" t="s">
         <v>1244</v>
       </c>
-      <c r="D467" t="s">
+      <c r="E467" t="s">
+        <v>49</v>
+      </c>
+      <c r="F467" t="s">
         <v>1245</v>
-      </c>
-      <c r="E467" t="s">
-        <v>49</v>
-      </c>
-      <c r="F467" t="s">
-        <v>1246</v>
       </c>
       <c r="G467" t="s">
         <v>203</v>
@@ -16363,10 +16360,10 @@
     </row>
     <row r="468" spans="1:12">
       <c r="B468" s="10" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C468" t="s">
         <v>1247</v>
-      </c>
-      <c r="C468" t="s">
-        <v>1248</v>
       </c>
       <c r="D468" t="s">
         <v>317</v>
@@ -16375,7 +16372,7 @@
         <v>49</v>
       </c>
       <c r="F468" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="G468" t="s">
         <v>317</v>
@@ -16386,10 +16383,10 @@
     </row>
     <row r="469" spans="1:12">
       <c r="B469" s="10" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C469" t="s">
         <v>1250</v>
-      </c>
-      <c r="C469" t="s">
-        <v>1251</v>
       </c>
       <c r="D469" t="s">
         <v>181</v>
@@ -16398,7 +16395,7 @@
         <v>49</v>
       </c>
       <c r="F469" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="G469" t="s">
         <v>181</v>
@@ -16409,19 +16406,19 @@
     </row>
     <row r="470" spans="1:12">
       <c r="B470" s="11" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C470" s="8" t="s">
         <v>1253</v>
       </c>
-      <c r="C470" s="8" t="s">
+      <c r="D470" s="8" t="s">
         <v>1254</v>
       </c>
-      <c r="D470" s="8" t="s">
+      <c r="E470" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F470" s="8" t="s">
         <v>1255</v>
-      </c>
-      <c r="E470" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F470" s="8" t="s">
-        <v>1256</v>
       </c>
       <c r="G470" s="8" t="s">
         <v>317</v>
@@ -16435,10 +16432,10 @@
         <v>13</v>
       </c>
       <c r="B471" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C471" t="s">
         <v>1257</v>
-      </c>
-      <c r="C471" t="s">
-        <v>1258</v>
       </c>
       <c r="D471" t="s">
         <v>436</v>
@@ -16465,7 +16462,7 @@
         <v>437</v>
       </c>
       <c r="L471" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="472" spans="1:12">
@@ -16493,10 +16490,10 @@
     </row>
     <row r="473" spans="1:12">
       <c r="B473" s="9" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C473" s="4" t="s">
         <v>1259</v>
-      </c>
-      <c r="C473" s="4" t="s">
-        <v>1260</v>
       </c>
       <c r="D473" s="4" t="s">
         <v>196</v>
@@ -16505,7 +16502,7 @@
         <v>49</v>
       </c>
       <c r="F473" s="4" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="G473" s="4" t="s">
         <v>196</v>
@@ -16516,10 +16513,10 @@
     </row>
     <row r="474" spans="1:12">
       <c r="B474" s="10" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C474" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="D474" t="s">
         <v>196</v>
@@ -16528,7 +16525,7 @@
         <v>49</v>
       </c>
       <c r="F474" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="G474" t="s">
         <v>196</v>
@@ -16539,10 +16536,10 @@
     </row>
     <row r="475" spans="1:12">
       <c r="B475" s="10" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C475" t="s">
         <v>1263</v>
-      </c>
-      <c r="C475" t="s">
-        <v>1264</v>
       </c>
       <c r="D475" t="s">
         <v>196</v>
@@ -16551,7 +16548,7 @@
         <v>49</v>
       </c>
       <c r="F475" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="G475" t="s">
         <v>196</v>
@@ -16562,19 +16559,19 @@
     </row>
     <row r="476" spans="1:12">
       <c r="B476" s="10" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C476" t="s">
         <v>1266</v>
       </c>
-      <c r="C476" t="s">
+      <c r="D476" t="s">
         <v>1267</v>
       </c>
-      <c r="D476" t="s">
+      <c r="E476" t="s">
+        <v>49</v>
+      </c>
+      <c r="F476" t="s">
         <v>1268</v>
-      </c>
-      <c r="E476" t="s">
-        <v>49</v>
-      </c>
-      <c r="F476" t="s">
-        <v>1269</v>
       </c>
       <c r="G476" t="s">
         <v>196</v>
@@ -16585,10 +16582,10 @@
     </row>
     <row r="477" spans="1:12">
       <c r="B477" s="10" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C477" t="s">
         <v>1270</v>
-      </c>
-      <c r="C477" t="s">
-        <v>1271</v>
       </c>
       <c r="D477" t="s">
         <v>196</v>
@@ -16597,7 +16594,7 @@
         <v>49</v>
       </c>
       <c r="F477" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="G477" t="s">
         <v>196</v>
@@ -16608,10 +16605,10 @@
     </row>
     <row r="478" spans="1:12">
       <c r="B478" s="11" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C478" s="8" t="s">
         <v>1273</v>
-      </c>
-      <c r="C478" s="8" t="s">
-        <v>1274</v>
       </c>
       <c r="D478" s="8" t="s">
         <v>196</v>
@@ -16620,7 +16617,7 @@
         <v>49</v>
       </c>
       <c r="F478" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="G478" s="8" t="s">
         <v>196</v>
@@ -16634,10 +16631,10 @@
         <v>13</v>
       </c>
       <c r="B479" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C479" t="s">
         <v>1276</v>
-      </c>
-      <c r="C479" t="s">
-        <v>1277</v>
       </c>
       <c r="D479" t="s">
         <v>436</v>
@@ -16664,7 +16661,7 @@
         <v>437</v>
       </c>
       <c r="L479" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="480" spans="1:12">
@@ -16692,19 +16689,19 @@
     </row>
     <row r="481" spans="1:12">
       <c r="B481" s="9" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C481" s="4" t="s">
         <v>1278</v>
       </c>
-      <c r="C481" s="4" t="s">
+      <c r="D481" s="4" t="s">
         <v>1279</v>
       </c>
-      <c r="D481" s="4" t="s">
+      <c r="E481" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F481" s="4" t="s">
         <v>1280</v>
-      </c>
-      <c r="E481" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F481" s="4" t="s">
-        <v>1281</v>
       </c>
       <c r="G481" s="4" t="s">
         <v>111</v>
@@ -16715,19 +16712,19 @@
     </row>
     <row r="482" spans="1:12">
       <c r="B482" s="10" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C482" t="s">
         <v>1282</v>
       </c>
-      <c r="C482" t="s">
-        <v>1283</v>
-      </c>
       <c r="D482" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E482" t="s">
+        <v>49</v>
+      </c>
+      <c r="F482" t="s">
         <v>1280</v>
-      </c>
-      <c r="E482" t="s">
-        <v>49</v>
-      </c>
-      <c r="F482" t="s">
-        <v>1281</v>
       </c>
       <c r="G482" t="s">
         <v>111</v>
@@ -16738,19 +16735,19 @@
     </row>
     <row r="483" spans="1:12">
       <c r="B483" s="10" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C483" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D483" t="s">
         <v>1279</v>
       </c>
-      <c r="D483" t="s">
+      <c r="E483" t="s">
+        <v>49</v>
+      </c>
+      <c r="F483" t="s">
         <v>1280</v>
-      </c>
-      <c r="E483" t="s">
-        <v>49</v>
-      </c>
-      <c r="F483" t="s">
-        <v>1281</v>
       </c>
       <c r="G483" t="s">
         <v>111</v>
@@ -16761,10 +16758,10 @@
     </row>
     <row r="484" spans="1:12">
       <c r="B484" s="10" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C484" t="s">
         <v>1285</v>
-      </c>
-      <c r="C484" t="s">
-        <v>1286</v>
       </c>
       <c r="D484" t="s">
         <v>111</v>
@@ -16773,7 +16770,7 @@
         <v>49</v>
       </c>
       <c r="F484" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="G484" t="s">
         <v>111</v>
@@ -16784,10 +16781,10 @@
     </row>
     <row r="485" spans="1:12">
       <c r="B485" s="10" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C485" t="s">
         <v>1288</v>
-      </c>
-      <c r="C485" t="s">
-        <v>1289</v>
       </c>
       <c r="D485" t="s">
         <v>111</v>
@@ -16796,7 +16793,7 @@
         <v>49</v>
       </c>
       <c r="F485" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="G485" t="s">
         <v>111</v>
@@ -16807,10 +16804,10 @@
     </row>
     <row r="486" spans="1:12">
       <c r="B486" s="10" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C486" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="D486" t="s">
         <v>111</v>
@@ -16819,7 +16816,7 @@
         <v>49</v>
       </c>
       <c r="F486" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="G486" t="s">
         <v>111</v>
@@ -16830,10 +16827,10 @@
     </row>
     <row r="487" spans="1:12">
       <c r="B487" s="10" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C487" t="s">
         <v>1292</v>
-      </c>
-      <c r="C487" t="s">
-        <v>1293</v>
       </c>
       <c r="D487" t="s">
         <v>111</v>
@@ -16842,7 +16839,7 @@
         <v>49</v>
       </c>
       <c r="F487" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="G487" t="s">
         <v>111</v>
@@ -16853,10 +16850,10 @@
     </row>
     <row r="488" spans="1:12">
       <c r="B488" s="10" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C488" t="s">
         <v>1295</v>
-      </c>
-      <c r="C488" t="s">
-        <v>1296</v>
       </c>
       <c r="D488" t="s">
         <v>111</v>
@@ -16865,7 +16862,7 @@
         <v>49</v>
       </c>
       <c r="F488" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="G488" t="s">
         <v>111</v>
@@ -16876,19 +16873,19 @@
     </row>
     <row r="489" spans="1:12">
       <c r="B489" s="11" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C489" s="8" t="s">
         <v>1298</v>
       </c>
-      <c r="C489" s="8" t="s">
+      <c r="D489" s="8" t="s">
         <v>1299</v>
       </c>
-      <c r="D489" s="8" t="s">
+      <c r="E489" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F489" s="8" t="s">
         <v>1300</v>
-      </c>
-      <c r="E489" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F489" s="8" t="s">
-        <v>1301</v>
       </c>
       <c r="G489" s="8" t="s">
         <v>111</v>
@@ -16902,10 +16899,10 @@
         <v>13</v>
       </c>
       <c r="B490" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C490" t="s">
         <v>1302</v>
-      </c>
-      <c r="C490" t="s">
-        <v>1303</v>
       </c>
       <c r="D490" t="s">
         <v>436</v>
@@ -16929,10 +16926,10 @@
         <v>39</v>
       </c>
       <c r="K490" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="L490" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="491" spans="1:12">
@@ -16960,19 +16957,19 @@
     </row>
     <row r="492" spans="1:12">
       <c r="B492" s="9" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C492" s="4" t="s">
         <v>1305</v>
       </c>
-      <c r="C492" s="4" t="s">
+      <c r="D492" s="4" t="s">
         <v>1306</v>
       </c>
-      <c r="D492" s="4" t="s">
+      <c r="E492" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F492" s="4" t="s">
         <v>1307</v>
-      </c>
-      <c r="E492" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F492" s="4" t="s">
-        <v>1308</v>
       </c>
       <c r="G492" s="4" t="s">
         <v>120</v>
@@ -16983,10 +16980,10 @@
     </row>
     <row r="493" spans="1:12">
       <c r="B493" s="10" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C493" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="D493" t="s">
         <v>120</v>
@@ -16995,7 +16992,7 @@
         <v>49</v>
       </c>
       <c r="F493" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="G493" t="s">
         <v>120</v>
@@ -17006,10 +17003,10 @@
     </row>
     <row r="494" spans="1:12">
       <c r="B494" s="10" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C494" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="D494" t="s">
         <v>120</v>
@@ -17018,7 +17015,7 @@
         <v>49</v>
       </c>
       <c r="F494" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G494" t="s">
         <v>120</v>
@@ -17029,10 +17026,10 @@
     </row>
     <row r="495" spans="1:12">
       <c r="B495" s="10" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C495" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="D495" t="s">
         <v>120</v>
@@ -17041,7 +17038,7 @@
         <v>49</v>
       </c>
       <c r="F495" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="G495" t="s">
         <v>120</v>
@@ -17052,10 +17049,10 @@
     </row>
     <row r="496" spans="1:12">
       <c r="B496" s="10" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C496" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="D496" t="s">
         <v>120</v>
@@ -17064,7 +17061,7 @@
         <v>49</v>
       </c>
       <c r="F496" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="G496" t="s">
         <v>120</v>
@@ -17075,10 +17072,10 @@
     </row>
     <row r="497" spans="1:12">
       <c r="B497" s="11" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C497" s="8" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="D497" s="8" t="s">
         <v>120</v>
@@ -17087,7 +17084,7 @@
         <v>49</v>
       </c>
       <c r="F497" s="8" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="G497" s="8" t="s">
         <v>120</v>
@@ -17101,10 +17098,10 @@
         <v>13</v>
       </c>
       <c r="B498" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C498" t="s">
         <v>1319</v>
-      </c>
-      <c r="C498" t="s">
-        <v>1320</v>
       </c>
       <c r="D498" t="s">
         <v>436</v>
@@ -17128,10 +17125,10 @@
         <v>57</v>
       </c>
       <c r="K498" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="L498" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="499" spans="1:12">
@@ -17159,19 +17156,19 @@
     </row>
     <row r="500" spans="1:12">
       <c r="B500" s="9" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C500" s="4" t="s">
         <v>1322</v>
       </c>
-      <c r="C500" s="4" t="s">
+      <c r="D500" s="4" t="s">
         <v>1323</v>
       </c>
-      <c r="D500" s="4" t="s">
+      <c r="E500" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F500" s="4" t="s">
         <v>1324</v>
-      </c>
-      <c r="E500" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F500" s="4" t="s">
-        <v>1325</v>
       </c>
       <c r="G500" s="4" t="s">
         <v>370</v>
@@ -17182,19 +17179,19 @@
     </row>
     <row r="501" spans="1:12">
       <c r="B501" s="10" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C501" t="s">
         <v>1326</v>
       </c>
-      <c r="C501" t="s">
+      <c r="D501" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E501" t="s">
+        <v>49</v>
+      </c>
+      <c r="F501" t="s">
         <v>1327</v>
-      </c>
-      <c r="D501" t="s">
-        <v>1324</v>
-      </c>
-      <c r="E501" t="s">
-        <v>49</v>
-      </c>
-      <c r="F501" t="s">
-        <v>1328</v>
       </c>
       <c r="G501" t="s">
         <v>370</v>
@@ -17205,19 +17202,19 @@
     </row>
     <row r="502" spans="1:12">
       <c r="B502" s="11" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="C502" s="8" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D502" s="8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E502" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F502" s="8" t="s">
         <v>1327</v>
-      </c>
-      <c r="D502" s="8" t="s">
-        <v>1324</v>
-      </c>
-      <c r="E502" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F502" s="8" t="s">
-        <v>1328</v>
       </c>
       <c r="G502" s="8" t="s">
         <v>370</v>
@@ -17231,10 +17228,10 @@
         <v>13</v>
       </c>
       <c r="B503" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C503" t="s">
         <v>1330</v>
-      </c>
-      <c r="C503" t="s">
-        <v>1331</v>
       </c>
       <c r="D503" t="s">
         <v>436</v>
@@ -17258,10 +17255,10 @@
         <v>39</v>
       </c>
       <c r="K503" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="L503" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="504" spans="1:12">
@@ -17289,10 +17286,10 @@
     </row>
     <row r="505" spans="1:12">
       <c r="B505" s="9" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C505" s="4" t="s">
         <v>1333</v>
-      </c>
-      <c r="C505" s="4" t="s">
-        <v>1334</v>
       </c>
       <c r="D505" s="4" t="s">
         <v>189</v>
@@ -17301,7 +17298,7 @@
         <v>49</v>
       </c>
       <c r="F505" s="4" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="G505" s="4" t="s">
         <v>189</v>
@@ -17312,19 +17309,19 @@
     </row>
     <row r="506" spans="1:12">
       <c r="B506" s="10" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C506" t="s">
         <v>1336</v>
       </c>
-      <c r="C506" t="s">
+      <c r="D506" t="s">
         <v>1337</v>
       </c>
-      <c r="D506" t="s">
+      <c r="E506" t="s">
+        <v>49</v>
+      </c>
+      <c r="F506" t="s">
         <v>1338</v>
-      </c>
-      <c r="E506" t="s">
-        <v>49</v>
-      </c>
-      <c r="F506" t="s">
-        <v>1339</v>
       </c>
       <c r="G506" t="s">
         <v>416</v>
@@ -17335,19 +17332,19 @@
     </row>
     <row r="507" spans="1:12">
       <c r="B507" s="10" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C507" t="s">
         <v>1340</v>
       </c>
-      <c r="C507" t="s">
+      <c r="D507" t="s">
         <v>1341</v>
       </c>
-      <c r="D507" t="s">
+      <c r="E507" t="s">
+        <v>49</v>
+      </c>
+      <c r="F507" t="s">
         <v>1342</v>
-      </c>
-      <c r="E507" t="s">
-        <v>49</v>
-      </c>
-      <c r="F507" t="s">
-        <v>1343</v>
       </c>
       <c r="G507" t="s">
         <v>416</v>
@@ -17358,19 +17355,19 @@
     </row>
     <row r="508" spans="1:12">
       <c r="B508" s="11" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C508" s="8" t="s">
         <v>1344</v>
       </c>
-      <c r="C508" s="8" t="s">
-        <v>1345</v>
-      </c>
       <c r="D508" s="8" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E508" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F508" s="8" t="s">
         <v>1342</v>
-      </c>
-      <c r="E508" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F508" s="8" t="s">
-        <v>1343</v>
       </c>
       <c r="G508" s="8" t="s">
         <v>416</v>
@@ -17384,10 +17381,10 @@
         <v>13</v>
       </c>
       <c r="B509" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C509" t="s">
         <v>1346</v>
-      </c>
-      <c r="C509" t="s">
-        <v>1347</v>
       </c>
       <c r="D509" t="s">
         <v>158</v>
@@ -17411,10 +17408,10 @@
         <v>57</v>
       </c>
       <c r="K509" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="L509" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="510" spans="1:12">
@@ -17442,10 +17439,10 @@
     </row>
     <row r="511" spans="1:12">
       <c r="B511" s="6" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C511" s="5" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="D511" s="5" t="s">
         <v>153</v>
@@ -17454,7 +17451,7 @@
         <v>49</v>
       </c>
       <c r="F511" s="5" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G511" s="5" t="s">
         <v>155</v>
@@ -17468,10 +17465,10 @@
         <v>13</v>
       </c>
       <c r="B512" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C512" t="s">
         <v>1350</v>
-      </c>
-      <c r="C512" t="s">
-        <v>1351</v>
       </c>
       <c r="D512" t="s">
         <v>158</v>
@@ -17498,7 +17495,7 @@
         <v>461</v>
       </c>
       <c r="L512" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="513" spans="1:12">
@@ -17526,10 +17523,10 @@
     </row>
     <row r="514" spans="1:12">
       <c r="B514" s="6" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="C514" s="5" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D514" s="5" t="s">
         <v>60</v>
@@ -17538,7 +17535,7 @@
         <v>49</v>
       </c>
       <c r="F514" s="5" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="G514" s="5" t="s">
         <v>60</v>
@@ -17552,10 +17549,10 @@
         <v>13</v>
       </c>
       <c r="B515" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C515" t="s">
         <v>1355</v>
-      </c>
-      <c r="C515" t="s">
-        <v>1356</v>
       </c>
       <c r="D515" t="s">
         <v>35</v>
@@ -17567,7 +17564,7 @@
         <v>379</v>
       </c>
       <c r="G515" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="H515" t="s">
         <v>134</v>
@@ -17579,10 +17576,10 @@
         <v>57</v>
       </c>
       <c r="K515" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L515" t="s">
         <v>1358</v>
-      </c>
-      <c r="L515" t="s">
-        <v>1359</v>
       </c>
     </row>
     <row r="516" spans="1:12">
@@ -17610,19 +17607,19 @@
     </row>
     <row r="517" spans="1:12">
       <c r="B517" s="6" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C517" s="5" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D517" s="5" t="s">
         <v>1360</v>
       </c>
-      <c r="D517" s="5" t="s">
+      <c r="E517" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F517" s="5" t="s">
         <v>1361</v>
-      </c>
-      <c r="E517" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F517" s="5" t="s">
-        <v>1362</v>
       </c>
       <c r="G517" s="5" t="s">
         <v>382</v>
@@ -17636,10 +17633,10 @@
         <v>13</v>
       </c>
       <c r="B518" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C518" t="s">
         <v>1363</v>
-      </c>
-      <c r="C518" t="s">
-        <v>1364</v>
       </c>
       <c r="D518" t="s">
         <v>35</v>
@@ -17651,7 +17648,7 @@
         <v>359</v>
       </c>
       <c r="G518" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="H518" t="s">
         <v>179</v>
@@ -17663,10 +17660,10 @@
         <v>57</v>
       </c>
       <c r="K518" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="L518" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="519" spans="1:12">
@@ -17694,19 +17691,19 @@
     </row>
     <row r="520" spans="1:12">
       <c r="B520" s="6" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C520" s="5" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D520" s="5" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E520" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F520" s="5" t="s">
         <v>1367</v>
-      </c>
-      <c r="D520" s="5" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E520" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F520" s="5" t="s">
-        <v>1368</v>
       </c>
       <c r="G520" s="5" t="s">
         <v>362</v>
@@ -17720,10 +17717,10 @@
         <v>13</v>
       </c>
       <c r="B521" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C521" t="s">
         <v>1369</v>
-      </c>
-      <c r="C521" t="s">
-        <v>1370</v>
       </c>
       <c r="D521" t="s">
         <v>35</v>
@@ -17735,7 +17732,7 @@
         <v>123</v>
       </c>
       <c r="G521" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="H521" t="s">
         <v>20</v>
@@ -17747,10 +17744,10 @@
         <v>57</v>
       </c>
       <c r="K521" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="L521" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="522" spans="1:12">
@@ -17778,10 +17775,10 @@
     </row>
     <row r="523" spans="1:12">
       <c r="B523" s="6" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="C523" s="5" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="D523" s="5" t="s">
         <v>129</v>
@@ -17790,7 +17787,7 @@
         <v>49</v>
       </c>
       <c r="F523" s="5" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="G523" s="5" t="s">
         <v>129</v>
@@ -17804,10 +17801,10 @@
         <v>13</v>
       </c>
       <c r="B524" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C524" t="s">
         <v>1375</v>
-      </c>
-      <c r="C524" t="s">
-        <v>1376</v>
       </c>
       <c r="D524" t="s">
         <v>35</v>
@@ -17819,7 +17816,7 @@
         <v>150</v>
       </c>
       <c r="G524" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="H524" t="s">
         <v>134</v>
@@ -17831,10 +17828,10 @@
         <v>57</v>
       </c>
       <c r="K524" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="L524" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="525" spans="1:12">
@@ -17862,10 +17859,10 @@
     </row>
     <row r="526" spans="1:12">
       <c r="B526" s="6" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="C526" s="5" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="D526" s="5" t="s">
         <v>153</v>
@@ -17874,7 +17871,7 @@
         <v>49</v>
       </c>
       <c r="F526" s="5" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G526" s="5" t="s">
         <v>155</v>
@@ -17888,10 +17885,10 @@
         <v>13</v>
       </c>
       <c r="B527" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C527" t="s">
         <v>1381</v>
-      </c>
-      <c r="C527" t="s">
-        <v>1382</v>
       </c>
       <c r="D527" t="s">
         <v>436</v>
@@ -17918,7 +17915,7 @@
         <v>437</v>
       </c>
       <c r="L527" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="528" spans="1:12" ht="15.6" thickTop="1" thickBot="1">
@@ -17960,10 +17957,10 @@
         <v>13</v>
       </c>
       <c r="B530" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C530" t="s">
         <v>1384</v>
-      </c>
-      <c r="C530" t="s">
-        <v>1385</v>
       </c>
       <c r="D530" t="s">
         <v>35</v>
@@ -17975,7 +17972,7 @@
         <v>308</v>
       </c>
       <c r="G530" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="H530" t="s">
         <v>38</v>
@@ -17990,7 +17987,7 @@
         <v>66</v>
       </c>
       <c r="L530" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="531" spans="1:12">
@@ -18018,19 +18015,19 @@
     </row>
     <row r="532" spans="1:12">
       <c r="B532" s="6" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C532" s="5" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D532" s="5" t="s">
         <v>1388</v>
       </c>
-      <c r="D532" s="5" t="s">
+      <c r="E532" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F532" s="5" t="s">
         <v>1389</v>
-      </c>
-      <c r="E532" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F532" s="5" t="s">
-        <v>1390</v>
       </c>
       <c r="G532" s="5" t="s">
         <v>310</v>
@@ -18044,10 +18041,10 @@
         <v>13</v>
       </c>
       <c r="B533" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C533" t="s">
         <v>1391</v>
-      </c>
-      <c r="C533" t="s">
-        <v>1392</v>
       </c>
       <c r="D533" t="s">
         <v>35</v>
@@ -18059,7 +18056,7 @@
         <v>200</v>
       </c>
       <c r="G533" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="H533" t="s">
         <v>20</v>
@@ -18074,7 +18071,7 @@
         <v>66</v>
       </c>
       <c r="L533" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="534" spans="1:12">
@@ -18102,19 +18099,19 @@
     </row>
     <row r="535" spans="1:12">
       <c r="B535" s="6" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C535" s="5" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D535" s="5" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E535" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F535" s="5" t="s">
         <v>1395</v>
-      </c>
-      <c r="D535" s="5" t="s">
-        <v>1245</v>
-      </c>
-      <c r="E535" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F535" s="5" t="s">
-        <v>1396</v>
       </c>
       <c r="G535" s="5" t="s">
         <v>203</v>

</xml_diff>

<commit_message>
added functionality for degenerate county names. Pre-SQL Join
</commit_message>
<xml_diff>
--- a/utility/data/HPSAdata/Hpsa_Find_Export (39).xlsx
+++ b/utility/data/HPSAdata/Hpsa_Find_Export (39).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsiu8\HPSA-Data\utility\data\HPSAdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D40F560-6DEF-441B-A0C1-654974FF0027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D45D64-5621-4EDF-89AD-02B7C45836C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="11928" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HPSA Find" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4101" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4102" uniqueCount="1396">
   <si>
     <t>data.HRSA.gov – HPSA Find</t>
   </si>
@@ -4405,22 +4405,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4739,8 +4739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
-      <selection activeCell="J319" sqref="J319"/>
+    <sheetView tabSelected="1" topLeftCell="A528" workbookViewId="0">
+      <selection activeCell="E530" sqref="E530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -17945,7 +17945,9 @@
       <c r="B529" s="6"/>
       <c r="C529" s="5"/>
       <c r="D529" s="5"/>
-      <c r="E529" s="5"/>
+      <c r="E529" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="F529" s="5"/>
       <c r="G529" s="5" t="s">
         <v>594</v>

</xml_diff>